<commit_message>
Tc updated with new tkt
</commit_message>
<xml_diff>
--- a/TCS_NEWUI_Carousel.xlsx
+++ b/TCS_NEWUI_Carousel.xlsx
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="292">
   <si>
     <t>Test Case Result Modules-Wise</t>
   </si>
@@ -903,6 +903,93 @@
     <t>1. Message "No items were found matching the parameters you've selected. Please try again by broadening your search." should be displayed
 2. Sorted by option should be removed from carousel</t>
   </si>
+  <si>
+    <t>US:WEB-7848_TC 01</t>
+  </si>
+  <si>
+    <t>Verify Carousel  when the default selected sorting option is First Run date</t>
+  </si>
+  <si>
+    <t>User should on Home screen of the application.
+Home screen should contain below section:
+1. Numerator logo on Top Left side of screen
+2. Report list on left side
+3. Total creatives chart
+4. Edit search list
+5. Search options
+6. Save and Reset button should be displayed as Disabled on Right side
+7. Export Result &amp; Search options button on Right bottom side</t>
+  </si>
+  <si>
+    <t>UA - Brand 
+ACC-QA  Testing Dashboard</t>
+  </si>
+  <si>
+    <t>Verify the default selected option of Sorted By below the Carousel</t>
+  </si>
+  <si>
+    <t>Default selected option for sorting of Carousel should be First Run Date</t>
+  </si>
+  <si>
+    <t>Verify the Carousel's Ad tile fields</t>
+  </si>
+  <si>
+    <t>1.User should be able to see the Media and First Run Date data on individual Ad tile</t>
+  </si>
+  <si>
+    <t>Verify All ads disaplyed in Carousel should be sorted by First Run Date data</t>
+  </si>
+  <si>
+    <t>User should be able to see that all the Ads in the Carousel are sorted in Descending order as per their First Run Date</t>
+  </si>
+  <si>
+    <t>US:WEB-7848_TC 02</t>
+  </si>
+  <si>
+    <t>Verify Carousel When user selects sorting option SPEND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Click on other Sorted by option i.e Spend </t>
+  </si>
+  <si>
+    <t>User should be able select the Spend radio button option</t>
+  </si>
+  <si>
+    <t>User should be able to see the Media and Spend data on individual Ad tile respectively</t>
+  </si>
+  <si>
+    <t>Verify All ads disaplyed in Carousel should be sorted by Spend data</t>
+  </si>
+  <si>
+    <t>User should be able to see that all the Ads in the Carousel are sorted in Descending order as per their Spend data</t>
+  </si>
+  <si>
+    <t>US:WEB-7848_TC 03</t>
+  </si>
+  <si>
+    <t>Verify the Carousel Ad tiles field by switching the sorting options</t>
+  </si>
+  <si>
+    <t>1.Default selected option for sorting of Carousel should be First Run Date
+2. Ads in the carousel should show the media and First Run Date data on it
+3. Ads should be sorted in descending order as per their First Run Date</t>
+  </si>
+  <si>
+    <t>Switch the selected option to Spend</t>
+  </si>
+  <si>
+    <t>1.Selected option for sorting of Carousel should be Spend now
+2. Ads in the carousel should show the media and Spend data on it
+3. Ads should be sorted in descending order as per their Spend data</t>
+  </si>
+  <si>
+    <t>Again Switch back to First Run Date option and observe the Ads in Carousel</t>
+  </si>
+  <si>
+    <t>1.User should be able to switch to First Run Date option for sorting of Carousel 
+2. Ads in the carousel should show the media and First Run Date data on it
+3. Ads should be sorted in descending order as per their First Run Date</t>
+  </si>
 </sst>
 </file>
 
@@ -911,11 +998,18 @@
   <numFmts count="1">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="52">
+  <fonts count="53">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1949,343 +2043,301 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
@@ -2294,380 +2346,423 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="34" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="33" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0">
+    <xf numFmtId="41" fontId="47" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="33" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="105">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="92" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="134"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="11" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="18" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="18" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="2" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="37" fillId="20" borderId="2" xfId="87" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="44" fillId="20" borderId="11" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="134" applyFont="1"/>
+    <xf numFmtId="9" fontId="39" fillId="4" borderId="19" xfId="143" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="12" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="46" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="0" borderId="0" xfId="152" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="46" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="32" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-  </cellStyleXfs>
-  <cellXfs count="104">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="0" xfId="92" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="134"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="153" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="19" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="20" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="23" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="24" xfId="143" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="25" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="143" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="27" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="28" xfId="143" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="23" borderId="20" xfId="143" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="23" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="143" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="25" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="27" borderId="32" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="28" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="33" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="34" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="35" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="36" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="153" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="153" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="37" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="38" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="143" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="11" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="18" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="18" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="4" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="2" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="36" fillId="20" borderId="2" xfId="87" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="10" fontId="43" fillId="20" borderId="11" xfId="138" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="134" applyFont="1"/>
-    <xf numFmtId="9" fontId="38" fillId="4" borderId="19" xfId="143" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="12" xfId="24" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="152" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="153" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="19" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="20" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="23" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="24" xfId="143" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="25" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="143" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="27" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="143" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="23" borderId="20" xfId="143" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="23" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="143" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="25" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="27" borderId="32" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="28" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="33" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="34" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="35" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="36" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="153" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="153" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="37" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="38" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="143" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="48" fillId="30" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="30" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="48" fillId="30" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="19" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="19" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="19" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="19" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="19" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="19" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="41" fontId="50" fillId="31" borderId="19" xfId="154" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="51" fillId="31" borderId="19" xfId="154" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="19" xfId="144" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="19" xfId="144" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="19" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="143" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="143" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="40" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="40" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="152" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="152" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="41" fontId="50" fillId="0" borderId="0" xfId="155" applyFont="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="51" fillId="0" borderId="0" xfId="155" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="42" fillId="0" borderId="0" xfId="146" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="43" fillId="0" borderId="0" xfId="146" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="146" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="146" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="146" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="146" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="152" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="152" applyFont="1">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="42" xfId="144" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="1" xfId="134" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="21" borderId="0" xfId="134" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="13" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="17" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="14" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="15" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="22" borderId="16" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="11" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="42" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="30" borderId="42" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="42" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="21" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="49" fillId="24" borderId="22" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="29" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="20" borderId="30" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="0" xfId="144" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="50" fillId="29" borderId="39" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="42" xfId="144" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="1" xfId="134" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="21" borderId="0" xfId="134" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="13" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="17" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="14" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="15" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="22" borderId="16" xfId="135" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="11" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="146" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="30" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="30" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="30" borderId="42" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="42" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="40" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="41" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="42" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="24" borderId="21" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="24" borderId="22" xfId="143" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="29" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="20" borderId="30" xfId="136" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="29" borderId="0" xfId="144" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="29" borderId="39" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="156">
     <cellStyle name="20% - Accent1" xfId="11"/>
@@ -2948,7 +3043,7 @@
           <c:x val="5.3923741222529187E-2"/>
           <c:y val="0.14185650994577867"/>
           <c:w val="0.90694002510216154"/>
-          <c:h val="0.75521895211321843"/>
+          <c:h val="0.75521895211321854"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3110,7 +3205,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3130,11 +3225,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="57193216"/>
-        <c:axId val="57194752"/>
+        <c:axId val="73763456"/>
+        <c:axId val="73773440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57193216"/>
+        <c:axId val="73763456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3153,14 +3248,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57194752"/>
+        <c:crossAx val="73773440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="57194752"/>
+        <c:axId val="73773440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3168,7 +3263,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="57193216"/>
+        <c:crossAx val="73763456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3188,7 +3283,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000522" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000522" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3234,8 +3329,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="3.8831278392536694E-2"/>
-          <c:y val="0.14624350369603387"/>
-          <c:w val="0.92496729254319732"/>
+          <c:y val="0.14624350369603392"/>
+          <c:w val="0.92496729254319754"/>
           <c:h val="0.69766331701963369"/>
         </c:manualLayout>
       </c:layout>
@@ -3348,10 +3443,10 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.95652173913043481</c:v>
+                  <c:v>0.96153846153846156</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.3478260869565188E-2</c:v>
+                  <c:v>3.8461538461538436E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3379,8 +3474,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.270891046791853"/>
-          <c:y val="0.88141746683253486"/>
-          <c:w val="0.42791036796598103"/>
+          <c:y val="0.88141746683253475"/>
+          <c:w val="0.4279103679659812"/>
           <c:h val="7.1280252974084315E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3400,7 +3495,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000366" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000366" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -3418,9 +3513,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.27595722641494741"/>
-          <c:y val="7.1365887012686383E-2"/>
-          <c:w val="0.29672375522792604"/>
-          <c:h val="0.85466509216403841"/>
+          <c:y val="7.1365887012686396E-2"/>
+          <c:w val="0.2967237552279261"/>
+          <c:h val="0.85466509216403863"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -3524,7 +3619,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>22</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3624,8 +3719,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.7216525124691745"/>
-          <c:y val="3.6083951617898588E-3"/>
+          <c:x val="0.72165251246917483"/>
+          <c:y val="3.6083951617898596E-3"/>
           <c:w val="0.24112408909611374"/>
           <c:h val="0.95693837006674254"/>
         </c:manualLayout>
@@ -3687,7 +3782,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000022" r="0.75000000000000022" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3713,7 +3808,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3751,7 +3846,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3789,7 +3884,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB276036-E4AE-4D63-9C65-0694CB3986A9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB276036-E4AE-4D63-9C65-0694CB3986A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3801,7 +3896,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3821,7 +3916,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3893,7 +3988,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AF65C03-9B72-4D6B-9DD9-6AFF172BC3B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5AF65C03-9B72-4D6B-9DD9-6AFF172BC3B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4027,7 +4122,7 @@
         </a:effectLst>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cmpd="sng">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4077,7 +4172,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E67F1DD6-8FFA-4013-AC77-D7090A499C80}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E67F1DD6-8FFA-4013-AC77-D7090A499C80}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4496,7 +4591,7 @@
       </c>
       <c r="B8" s="12">
         <f>'SMART- Carousel'!G7</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C8" s="12">
         <f>'SMART- Carousel'!G8</f>
@@ -4512,11 +4607,11 @@
       </c>
       <c r="F8" s="12">
         <f>SUM(B8:E8)</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G8" s="17">
         <f>(B8+C8+D8)/(F8)</f>
-        <v>0.95652173913043481</v>
+        <v>0.96153846153846156</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4534,7 +4629,7 @@
       </c>
       <c r="B10" s="18">
         <f>SUM(B8:B9)</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C10" s="18">
         <f>SUM(C8:C9)</f>
@@ -4550,11 +4645,11 @@
       </c>
       <c r="F10" s="18">
         <f>SUM(F8:F9)</f>
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G10" s="14">
         <f>SUM(G8:G8)</f>
-        <v>0.95652173913043481</v>
+        <v>0.96153846153846156</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickTop="1">
@@ -4563,7 +4658,7 @@
       </c>
       <c r="G11" s="15">
         <f>100%-G10</f>
-        <v>4.3478260869565188E-2</v>
+        <v>3.8461538461538436E-2</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -5492,7 +5587,7 @@
   <mergeCells count="1">
     <mergeCell ref="A2:A45"/>
   </mergeCells>
-  <phoneticPr fontId="44" type="noConversion"/>
+  <phoneticPr fontId="45" type="noConversion"/>
   <pageMargins left="0.69861111111111107" right="0.69861111111111107" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -5503,8 +5598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H960"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A263" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B272" sqref="B272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -6250,7 +6345,7 @@
       </c>
       <c r="G7" s="37">
         <f>COUNTIF(G11:G1086,"Pass")</f>
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickBot="1">
@@ -6310,7 +6405,7 @@
       </c>
       <c r="C11" s="28">
         <f>G7</f>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D11"/>
       <c r="E11" s="26"/>
@@ -6389,12 +6484,12 @@
       <c r="A18" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="89" t="s">
+      <c r="B18" s="92" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="90"/>
-      <c r="D18" s="90"/>
-      <c r="E18" s="91"/>
+      <c r="C18" s="93"/>
+      <c r="D18" s="93"/>
+      <c r="E18" s="94"/>
       <c r="F18" s="51" t="s">
         <v>46</v>
       </c>
@@ -6407,14 +6502,14 @@
       <c r="A19" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="92" t="s">
+      <c r="B19" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="93"/>
-      <c r="D19" s="93"/>
-      <c r="E19" s="93"/>
-      <c r="F19" s="93"/>
-      <c r="G19" s="94"/>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="96"/>
+      <c r="F19" s="96"/>
+      <c r="G19" s="97"/>
     </row>
     <row r="20" spans="1:7" s="49" customFormat="1">
       <c r="A20" s="54" t="s">
@@ -6479,23 +6574,23 @@
       <c r="A23" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="95"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
-      <c r="F23" s="96"/>
-      <c r="G23" s="97"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="90"/>
+      <c r="D23" s="90"/>
+      <c r="E23" s="90"/>
+      <c r="F23" s="90"/>
+      <c r="G23" s="91"/>
     </row>
     <row r="24" spans="1:7" s="49" customFormat="1">
       <c r="A24" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="89" t="s">
+      <c r="B24" s="92" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="90"/>
-      <c r="D24" s="90"/>
-      <c r="E24" s="91"/>
+      <c r="C24" s="93"/>
+      <c r="D24" s="93"/>
+      <c r="E24" s="94"/>
       <c r="F24" s="51" t="s">
         <v>46</v>
       </c>
@@ -6508,14 +6603,14 @@
       <c r="A25" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="92" t="s">
+      <c r="B25" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="93"/>
-      <c r="D25" s="93"/>
-      <c r="E25" s="93"/>
-      <c r="F25" s="93"/>
-      <c r="G25" s="94"/>
+      <c r="C25" s="96"/>
+      <c r="D25" s="96"/>
+      <c r="E25" s="96"/>
+      <c r="F25" s="96"/>
+      <c r="G25" s="97"/>
     </row>
     <row r="26" spans="1:7" s="49" customFormat="1">
       <c r="A26" s="54" t="s">
@@ -6595,23 +6690,23 @@
       <c r="A30" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="95"/>
-      <c r="C30" s="96"/>
-      <c r="D30" s="96"/>
-      <c r="E30" s="96"/>
-      <c r="F30" s="96"/>
-      <c r="G30" s="97"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="90"/>
+      <c r="D30" s="90"/>
+      <c r="E30" s="90"/>
+      <c r="F30" s="90"/>
+      <c r="G30" s="91"/>
     </row>
     <row r="31" spans="1:7" s="49" customFormat="1">
       <c r="A31" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="89" t="s">
+      <c r="B31" s="92" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="90"/>
-      <c r="D31" s="90"/>
-      <c r="E31" s="91"/>
+      <c r="C31" s="93"/>
+      <c r="D31" s="93"/>
+      <c r="E31" s="94"/>
       <c r="F31" s="51" t="s">
         <v>46</v>
       </c>
@@ -6624,14 +6719,14 @@
       <c r="A32" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="92" t="s">
+      <c r="B32" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="93"/>
-      <c r="D32" s="93"/>
-      <c r="E32" s="93"/>
-      <c r="F32" s="93"/>
-      <c r="G32" s="94"/>
+      <c r="C32" s="96"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="96"/>
+      <c r="F32" s="96"/>
+      <c r="G32" s="97"/>
     </row>
     <row r="33" spans="1:7" s="49" customFormat="1">
       <c r="A33" s="54" t="s">
@@ -6728,23 +6823,23 @@
       <c r="A38" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="95"/>
-      <c r="C38" s="96"/>
-      <c r="D38" s="96"/>
-      <c r="E38" s="96"/>
-      <c r="F38" s="96"/>
-      <c r="G38" s="97"/>
+      <c r="B38" s="89"/>
+      <c r="C38" s="90"/>
+      <c r="D38" s="90"/>
+      <c r="E38" s="90"/>
+      <c r="F38" s="90"/>
+      <c r="G38" s="91"/>
     </row>
     <row r="39" spans="1:7" s="49" customFormat="1">
       <c r="A39" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="B39" s="89" t="s">
+      <c r="B39" s="92" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="90"/>
-      <c r="D39" s="90"/>
-      <c r="E39" s="91"/>
+      <c r="C39" s="93"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="94"/>
       <c r="F39" s="51" t="s">
         <v>46</v>
       </c>
@@ -6757,14 +6852,14 @@
       <c r="A40" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="92" t="s">
+      <c r="B40" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="93"/>
-      <c r="D40" s="93"/>
-      <c r="E40" s="93"/>
-      <c r="F40" s="93"/>
-      <c r="G40" s="94"/>
+      <c r="C40" s="96"/>
+      <c r="D40" s="96"/>
+      <c r="E40" s="96"/>
+      <c r="F40" s="96"/>
+      <c r="G40" s="97"/>
     </row>
     <row r="41" spans="1:7" s="49" customFormat="1">
       <c r="A41" s="54" t="s">
@@ -6861,23 +6956,23 @@
       <c r="A46" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="95"/>
-      <c r="C46" s="96"/>
-      <c r="D46" s="96"/>
-      <c r="E46" s="96"/>
-      <c r="F46" s="96"/>
-      <c r="G46" s="97"/>
+      <c r="B46" s="89"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="90"/>
+      <c r="F46" s="90"/>
+      <c r="G46" s="91"/>
     </row>
     <row r="47" spans="1:7" s="49" customFormat="1">
       <c r="A47" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="B47" s="89" t="s">
+      <c r="B47" s="92" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="90"/>
-      <c r="D47" s="90"/>
-      <c r="E47" s="91"/>
+      <c r="C47" s="93"/>
+      <c r="D47" s="93"/>
+      <c r="E47" s="94"/>
       <c r="F47" s="51" t="s">
         <v>46</v>
       </c>
@@ -6890,14 +6985,14 @@
       <c r="A48" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="92" t="s">
+      <c r="B48" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="93"/>
-      <c r="D48" s="93"/>
-      <c r="E48" s="93"/>
-      <c r="F48" s="93"/>
-      <c r="G48" s="94"/>
+      <c r="C48" s="96"/>
+      <c r="D48" s="96"/>
+      <c r="E48" s="96"/>
+      <c r="F48" s="96"/>
+      <c r="G48" s="97"/>
     </row>
     <row r="49" spans="1:7" s="49" customFormat="1">
       <c r="A49" s="54" t="s">
@@ -6994,23 +7089,23 @@
       <c r="A54" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="95"/>
-      <c r="C54" s="96"/>
-      <c r="D54" s="96"/>
-      <c r="E54" s="96"/>
-      <c r="F54" s="96"/>
-      <c r="G54" s="97"/>
+      <c r="B54" s="89"/>
+      <c r="C54" s="90"/>
+      <c r="D54" s="90"/>
+      <c r="E54" s="90"/>
+      <c r="F54" s="90"/>
+      <c r="G54" s="91"/>
     </row>
     <row r="55" spans="1:7" s="49" customFormat="1">
       <c r="A55" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="89" t="s">
+      <c r="B55" s="92" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="90"/>
-      <c r="D55" s="90"/>
-      <c r="E55" s="91"/>
+      <c r="C55" s="93"/>
+      <c r="D55" s="93"/>
+      <c r="E55" s="94"/>
       <c r="F55" s="51" t="s">
         <v>46</v>
       </c>
@@ -7023,14 +7118,14 @@
       <c r="A56" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="92" t="s">
+      <c r="B56" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="93"/>
-      <c r="D56" s="93"/>
-      <c r="E56" s="93"/>
-      <c r="F56" s="93"/>
-      <c r="G56" s="94"/>
+      <c r="C56" s="96"/>
+      <c r="D56" s="96"/>
+      <c r="E56" s="96"/>
+      <c r="F56" s="96"/>
+      <c r="G56" s="97"/>
     </row>
     <row r="57" spans="1:7" s="49" customFormat="1">
       <c r="A57" s="54" t="s">
@@ -7127,23 +7222,23 @@
       <c r="A62" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="95"/>
-      <c r="C62" s="96"/>
-      <c r="D62" s="96"/>
-      <c r="E62" s="96"/>
-      <c r="F62" s="96"/>
-      <c r="G62" s="97"/>
+      <c r="B62" s="89"/>
+      <c r="C62" s="90"/>
+      <c r="D62" s="90"/>
+      <c r="E62" s="90"/>
+      <c r="F62" s="90"/>
+      <c r="G62" s="91"/>
     </row>
     <row r="63" spans="1:7" s="49" customFormat="1">
       <c r="A63" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="89" t="s">
+      <c r="B63" s="92" t="s">
         <v>70</v>
       </c>
-      <c r="C63" s="90"/>
-      <c r="D63" s="90"/>
-      <c r="E63" s="91"/>
+      <c r="C63" s="93"/>
+      <c r="D63" s="93"/>
+      <c r="E63" s="94"/>
       <c r="F63" s="51" t="s">
         <v>46</v>
       </c>
@@ -7156,14 +7251,14 @@
       <c r="A64" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B64" s="92" t="s">
+      <c r="B64" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C64" s="93"/>
-      <c r="D64" s="93"/>
-      <c r="E64" s="93"/>
-      <c r="F64" s="93"/>
-      <c r="G64" s="94"/>
+      <c r="C64" s="96"/>
+      <c r="D64" s="96"/>
+      <c r="E64" s="96"/>
+      <c r="F64" s="96"/>
+      <c r="G64" s="97"/>
     </row>
     <row r="65" spans="1:7" s="49" customFormat="1">
       <c r="A65" s="54" t="s">
@@ -7260,23 +7355,23 @@
       <c r="A70" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B70" s="95"/>
-      <c r="C70" s="96"/>
-      <c r="D70" s="96"/>
-      <c r="E70" s="96"/>
-      <c r="F70" s="96"/>
-      <c r="G70" s="97"/>
+      <c r="B70" s="89"/>
+      <c r="C70" s="90"/>
+      <c r="D70" s="90"/>
+      <c r="E70" s="90"/>
+      <c r="F70" s="90"/>
+      <c r="G70" s="91"/>
     </row>
     <row r="71" spans="1:7" s="49" customFormat="1">
       <c r="A71" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="B71" s="89" t="s">
+      <c r="B71" s="92" t="s">
         <v>92</v>
       </c>
-      <c r="C71" s="90"/>
-      <c r="D71" s="90"/>
-      <c r="E71" s="91"/>
+      <c r="C71" s="93"/>
+      <c r="D71" s="93"/>
+      <c r="E71" s="94"/>
       <c r="F71" s="51" t="s">
         <v>46</v>
       </c>
@@ -7289,14 +7384,14 @@
       <c r="A72" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B72" s="92" t="s">
+      <c r="B72" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C72" s="93"/>
-      <c r="D72" s="93"/>
-      <c r="E72" s="93"/>
-      <c r="F72" s="93"/>
-      <c r="G72" s="94"/>
+      <c r="C72" s="96"/>
+      <c r="D72" s="96"/>
+      <c r="E72" s="96"/>
+      <c r="F72" s="96"/>
+      <c r="G72" s="97"/>
     </row>
     <row r="73" spans="1:7" s="49" customFormat="1">
       <c r="A73" s="54" t="s">
@@ -7393,23 +7488,23 @@
       <c r="A78" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B78" s="95"/>
-      <c r="C78" s="96"/>
-      <c r="D78" s="96"/>
-      <c r="E78" s="96"/>
-      <c r="F78" s="96"/>
-      <c r="G78" s="97"/>
+      <c r="B78" s="89"/>
+      <c r="C78" s="90"/>
+      <c r="D78" s="90"/>
+      <c r="E78" s="90"/>
+      <c r="F78" s="90"/>
+      <c r="G78" s="91"/>
     </row>
     <row r="79" spans="1:7" s="49" customFormat="1">
       <c r="A79" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="B79" s="89" t="s">
+      <c r="B79" s="92" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="90"/>
-      <c r="D79" s="90"/>
-      <c r="E79" s="91"/>
+      <c r="C79" s="93"/>
+      <c r="D79" s="93"/>
+      <c r="E79" s="94"/>
       <c r="F79" s="51" t="s">
         <v>46</v>
       </c>
@@ -7422,14 +7517,14 @@
       <c r="A80" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B80" s="92" t="s">
+      <c r="B80" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C80" s="93"/>
-      <c r="D80" s="93"/>
-      <c r="E80" s="93"/>
-      <c r="F80" s="93"/>
-      <c r="G80" s="94"/>
+      <c r="C80" s="96"/>
+      <c r="D80" s="96"/>
+      <c r="E80" s="96"/>
+      <c r="F80" s="96"/>
+      <c r="G80" s="97"/>
     </row>
     <row r="81" spans="1:7" s="49" customFormat="1">
       <c r="A81" s="54" t="s">
@@ -7611,23 +7706,23 @@
       <c r="A91" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B91" s="95"/>
-      <c r="C91" s="96"/>
-      <c r="D91" s="96"/>
-      <c r="E91" s="96"/>
-      <c r="F91" s="96"/>
-      <c r="G91" s="97"/>
+      <c r="B91" s="89"/>
+      <c r="C91" s="90"/>
+      <c r="D91" s="90"/>
+      <c r="E91" s="90"/>
+      <c r="F91" s="90"/>
+      <c r="G91" s="91"/>
     </row>
     <row r="92" spans="1:7" customFormat="1">
       <c r="A92" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="B92" s="89" t="s">
+      <c r="B92" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="90"/>
-      <c r="D92" s="90"/>
-      <c r="E92" s="91"/>
+      <c r="C92" s="93"/>
+      <c r="D92" s="93"/>
+      <c r="E92" s="94"/>
       <c r="F92" s="51" t="s">
         <v>46</v>
       </c>
@@ -7640,14 +7735,14 @@
       <c r="A93" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B93" s="92" t="s">
+      <c r="B93" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C93" s="93"/>
-      <c r="D93" s="93"/>
-      <c r="E93" s="93"/>
-      <c r="F93" s="93"/>
-      <c r="G93" s="94"/>
+      <c r="C93" s="96"/>
+      <c r="D93" s="96"/>
+      <c r="E93" s="96"/>
+      <c r="F93" s="96"/>
+      <c r="G93" s="97"/>
     </row>
     <row r="94" spans="1:7" customFormat="1">
       <c r="A94" s="54" t="s">
@@ -7846,23 +7941,23 @@
       <c r="A105" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B105" s="95"/>
-      <c r="C105" s="96"/>
-      <c r="D105" s="96"/>
-      <c r="E105" s="96"/>
-      <c r="F105" s="96"/>
-      <c r="G105" s="97"/>
+      <c r="B105" s="89"/>
+      <c r="C105" s="90"/>
+      <c r="D105" s="90"/>
+      <c r="E105" s="90"/>
+      <c r="F105" s="90"/>
+      <c r="G105" s="91"/>
     </row>
     <row r="106" spans="1:7" customFormat="1">
       <c r="A106" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="B106" s="89" t="s">
+      <c r="B106" s="92" t="s">
         <v>89</v>
       </c>
-      <c r="C106" s="90"/>
-      <c r="D106" s="90"/>
-      <c r="E106" s="91"/>
+      <c r="C106" s="93"/>
+      <c r="D106" s="93"/>
+      <c r="E106" s="94"/>
       <c r="F106" s="51" t="s">
         <v>46</v>
       </c>
@@ -7875,14 +7970,14 @@
       <c r="A107" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B107" s="92" t="s">
+      <c r="B107" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C107" s="93"/>
-      <c r="D107" s="93"/>
-      <c r="E107" s="93"/>
-      <c r="F107" s="93"/>
-      <c r="G107" s="94"/>
+      <c r="C107" s="96"/>
+      <c r="D107" s="96"/>
+      <c r="E107" s="96"/>
+      <c r="F107" s="96"/>
+      <c r="G107" s="97"/>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="54" t="s">
@@ -8064,23 +8159,23 @@
       <c r="A118" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B118" s="95"/>
-      <c r="C118" s="96"/>
-      <c r="D118" s="96"/>
-      <c r="E118" s="96"/>
-      <c r="F118" s="96"/>
-      <c r="G118" s="97"/>
+      <c r="B118" s="89"/>
+      <c r="C118" s="90"/>
+      <c r="D118" s="90"/>
+      <c r="E118" s="90"/>
+      <c r="F118" s="90"/>
+      <c r="G118" s="91"/>
     </row>
     <row r="119" spans="1:8">
       <c r="A119" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="B119" s="89" t="s">
+      <c r="B119" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="C119" s="90"/>
-      <c r="D119" s="90"/>
-      <c r="E119" s="91"/>
+      <c r="C119" s="93"/>
+      <c r="D119" s="93"/>
+      <c r="E119" s="94"/>
       <c r="F119" s="51" t="s">
         <v>46</v>
       </c>
@@ -8093,14 +8188,14 @@
       <c r="A120" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B120" s="92" t="s">
+      <c r="B120" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C120" s="93"/>
-      <c r="D120" s="93"/>
-      <c r="E120" s="93"/>
-      <c r="F120" s="93"/>
-      <c r="G120" s="94"/>
+      <c r="C120" s="96"/>
+      <c r="D120" s="96"/>
+      <c r="E120" s="96"/>
+      <c r="F120" s="96"/>
+      <c r="G120" s="97"/>
       <c r="H120" s="63"/>
     </row>
     <row r="121" spans="1:8">
@@ -8300,23 +8395,23 @@
       <c r="A132" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B132" s="95"/>
-      <c r="C132" s="96"/>
-      <c r="D132" s="96"/>
-      <c r="E132" s="96"/>
-      <c r="F132" s="96"/>
-      <c r="G132" s="97"/>
+      <c r="B132" s="89"/>
+      <c r="C132" s="90"/>
+      <c r="D132" s="90"/>
+      <c r="E132" s="90"/>
+      <c r="F132" s="90"/>
+      <c r="G132" s="91"/>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="B133" s="89" t="s">
+      <c r="B133" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C133" s="90"/>
-      <c r="D133" s="90"/>
-      <c r="E133" s="91"/>
+      <c r="C133" s="93"/>
+      <c r="D133" s="93"/>
+      <c r="E133" s="94"/>
       <c r="F133" s="51" t="s">
         <v>46</v>
       </c>
@@ -8329,14 +8424,14 @@
       <c r="A134" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B134" s="92" t="s">
+      <c r="B134" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C134" s="93"/>
-      <c r="D134" s="93"/>
-      <c r="E134" s="93"/>
-      <c r="F134" s="93"/>
-      <c r="G134" s="94"/>
+      <c r="C134" s="96"/>
+      <c r="D134" s="96"/>
+      <c r="E134" s="96"/>
+      <c r="F134" s="96"/>
+      <c r="G134" s="97"/>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="54" t="s">
@@ -8535,23 +8630,23 @@
       <c r="A146" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B146" s="95"/>
-      <c r="C146" s="96"/>
-      <c r="D146" s="96"/>
-      <c r="E146" s="96"/>
-      <c r="F146" s="96"/>
-      <c r="G146" s="97"/>
+      <c r="B146" s="89"/>
+      <c r="C146" s="90"/>
+      <c r="D146" s="90"/>
+      <c r="E146" s="90"/>
+      <c r="F146" s="90"/>
+      <c r="G146" s="91"/>
     </row>
     <row r="147" spans="1:7">
       <c r="A147" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="B147" s="89" t="s">
+      <c r="B147" s="92" t="s">
         <v>86</v>
       </c>
-      <c r="C147" s="90"/>
-      <c r="D147" s="90"/>
-      <c r="E147" s="91"/>
+      <c r="C147" s="93"/>
+      <c r="D147" s="93"/>
+      <c r="E147" s="94"/>
       <c r="F147" s="51" t="s">
         <v>46</v>
       </c>
@@ -8564,14 +8659,14 @@
       <c r="A148" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B148" s="92" t="s">
+      <c r="B148" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C148" s="93"/>
-      <c r="D148" s="93"/>
-      <c r="E148" s="93"/>
-      <c r="F148" s="93"/>
-      <c r="G148" s="94"/>
+      <c r="C148" s="96"/>
+      <c r="D148" s="96"/>
+      <c r="E148" s="96"/>
+      <c r="F148" s="96"/>
+      <c r="G148" s="97"/>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" s="54" t="s">
@@ -8787,23 +8882,23 @@
       <c r="A161" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B161" s="95"/>
-      <c r="C161" s="96"/>
-      <c r="D161" s="96"/>
-      <c r="E161" s="96"/>
-      <c r="F161" s="96"/>
-      <c r="G161" s="97"/>
+      <c r="B161" s="89"/>
+      <c r="C161" s="90"/>
+      <c r="D161" s="90"/>
+      <c r="E161" s="90"/>
+      <c r="F161" s="90"/>
+      <c r="G161" s="91"/>
     </row>
     <row r="162" spans="1:7">
       <c r="A162" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="B162" s="89" t="s">
+      <c r="B162" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="C162" s="90"/>
-      <c r="D162" s="90"/>
-      <c r="E162" s="91"/>
+      <c r="C162" s="93"/>
+      <c r="D162" s="93"/>
+      <c r="E162" s="94"/>
       <c r="F162" s="51" t="s">
         <v>46</v>
       </c>
@@ -8816,14 +8911,14 @@
       <c r="A163" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B163" s="92" t="s">
+      <c r="B163" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C163" s="93"/>
-      <c r="D163" s="93"/>
-      <c r="E163" s="93"/>
-      <c r="F163" s="93"/>
-      <c r="G163" s="94"/>
+      <c r="C163" s="96"/>
+      <c r="D163" s="96"/>
+      <c r="E163" s="96"/>
+      <c r="F163" s="96"/>
+      <c r="G163" s="97"/>
     </row>
     <row r="164" spans="1:7" ht="30.95" customHeight="1">
       <c r="A164" s="54" t="s">
@@ -9022,23 +9117,23 @@
       <c r="A175" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B175" s="95"/>
-      <c r="C175" s="96"/>
-      <c r="D175" s="96"/>
-      <c r="E175" s="96"/>
-      <c r="F175" s="96"/>
-      <c r="G175" s="97"/>
+      <c r="B175" s="89"/>
+      <c r="C175" s="90"/>
+      <c r="D175" s="90"/>
+      <c r="E175" s="90"/>
+      <c r="F175" s="90"/>
+      <c r="G175" s="91"/>
     </row>
     <row r="176" spans="1:7">
       <c r="A176" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="B176" s="89" t="s">
+      <c r="B176" s="92" t="s">
         <v>84</v>
       </c>
-      <c r="C176" s="90"/>
-      <c r="D176" s="90"/>
-      <c r="E176" s="91"/>
+      <c r="C176" s="93"/>
+      <c r="D176" s="93"/>
+      <c r="E176" s="94"/>
       <c r="F176" s="51" t="s">
         <v>46</v>
       </c>
@@ -9051,14 +9146,14 @@
       <c r="A177" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B177" s="92" t="s">
+      <c r="B177" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C177" s="93"/>
-      <c r="D177" s="93"/>
-      <c r="E177" s="93"/>
-      <c r="F177" s="93"/>
-      <c r="G177" s="94"/>
+      <c r="C177" s="96"/>
+      <c r="D177" s="96"/>
+      <c r="E177" s="96"/>
+      <c r="F177" s="96"/>
+      <c r="G177" s="97"/>
     </row>
     <row r="178" spans="1:7">
       <c r="A178" s="54" t="s">
@@ -9274,23 +9369,23 @@
       <c r="A190" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B190" s="95"/>
-      <c r="C190" s="96"/>
-      <c r="D190" s="96"/>
-      <c r="E190" s="96"/>
-      <c r="F190" s="96"/>
-      <c r="G190" s="97"/>
+      <c r="B190" s="89"/>
+      <c r="C190" s="90"/>
+      <c r="D190" s="90"/>
+      <c r="E190" s="90"/>
+      <c r="F190" s="90"/>
+      <c r="G190" s="91"/>
     </row>
     <row r="191" spans="1:7">
       <c r="A191" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="89" t="s">
+      <c r="B191" s="92" t="s">
         <v>203</v>
       </c>
-      <c r="C191" s="90"/>
-      <c r="D191" s="90"/>
-      <c r="E191" s="91"/>
+      <c r="C191" s="93"/>
+      <c r="D191" s="93"/>
+      <c r="E191" s="94"/>
       <c r="F191" s="51" t="s">
         <v>46</v>
       </c>
@@ -9303,14 +9398,14 @@
       <c r="A192" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B192" s="92" t="s">
+      <c r="B192" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C192" s="93"/>
-      <c r="D192" s="93"/>
-      <c r="E192" s="93"/>
-      <c r="F192" s="93"/>
-      <c r="G192" s="94"/>
+      <c r="C192" s="96"/>
+      <c r="D192" s="96"/>
+      <c r="E192" s="96"/>
+      <c r="F192" s="96"/>
+      <c r="G192" s="97"/>
     </row>
     <row r="193" spans="1:7">
       <c r="A193" s="54" t="s">
@@ -9594,23 +9689,23 @@
       <c r="A209" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B209" s="95"/>
-      <c r="C209" s="96"/>
-      <c r="D209" s="96"/>
-      <c r="E209" s="96"/>
-      <c r="F209" s="96"/>
-      <c r="G209" s="97"/>
+      <c r="B209" s="89"/>
+      <c r="C209" s="90"/>
+      <c r="D209" s="90"/>
+      <c r="E209" s="90"/>
+      <c r="F209" s="90"/>
+      <c r="G209" s="91"/>
     </row>
     <row r="210" spans="1:7">
       <c r="A210" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="B210" s="89" t="s">
+      <c r="B210" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="C210" s="90"/>
-      <c r="D210" s="90"/>
-      <c r="E210" s="91"/>
+      <c r="C210" s="93"/>
+      <c r="D210" s="93"/>
+      <c r="E210" s="94"/>
       <c r="F210" s="51" t="s">
         <v>46</v>
       </c>
@@ -9623,14 +9718,14 @@
       <c r="A211" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B211" s="92" t="s">
+      <c r="B211" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C211" s="93"/>
-      <c r="D211" s="93"/>
-      <c r="E211" s="93"/>
-      <c r="F211" s="93"/>
-      <c r="G211" s="94"/>
+      <c r="C211" s="96"/>
+      <c r="D211" s="96"/>
+      <c r="E211" s="96"/>
+      <c r="F211" s="96"/>
+      <c r="G211" s="97"/>
     </row>
     <row r="212" spans="1:7">
       <c r="A212" s="54" t="s">
@@ -9761,23 +9856,23 @@
       <c r="A219" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B219" s="95"/>
-      <c r="C219" s="96"/>
-      <c r="D219" s="96"/>
-      <c r="E219" s="96"/>
-      <c r="F219" s="96"/>
-      <c r="G219" s="97"/>
+      <c r="B219" s="89"/>
+      <c r="C219" s="90"/>
+      <c r="D219" s="90"/>
+      <c r="E219" s="90"/>
+      <c r="F219" s="90"/>
+      <c r="G219" s="91"/>
     </row>
     <row r="220" spans="1:7">
       <c r="A220" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="B220" s="89" t="s">
+      <c r="B220" s="92" t="s">
         <v>252</v>
       </c>
-      <c r="C220" s="90"/>
-      <c r="D220" s="90"/>
-      <c r="E220" s="91"/>
+      <c r="C220" s="93"/>
+      <c r="D220" s="93"/>
+      <c r="E220" s="94"/>
       <c r="F220" s="51" t="s">
         <v>46</v>
       </c>
@@ -9790,14 +9885,14 @@
       <c r="A221" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B221" s="92" t="s">
+      <c r="B221" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C221" s="93"/>
-      <c r="D221" s="93"/>
-      <c r="E221" s="93"/>
-      <c r="F221" s="93"/>
-      <c r="G221" s="94"/>
+      <c r="C221" s="96"/>
+      <c r="D221" s="96"/>
+      <c r="E221" s="96"/>
+      <c r="F221" s="96"/>
+      <c r="G221" s="97"/>
     </row>
     <row r="222" spans="1:7">
       <c r="A222" s="54" t="s">
@@ -9985,23 +10080,23 @@
       <c r="A232" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B232" s="95"/>
-      <c r="C232" s="96"/>
-      <c r="D232" s="96"/>
-      <c r="E232" s="96"/>
-      <c r="F232" s="96"/>
-      <c r="G232" s="97"/>
+      <c r="B232" s="89"/>
+      <c r="C232" s="90"/>
+      <c r="D232" s="90"/>
+      <c r="E232" s="90"/>
+      <c r="F232" s="90"/>
+      <c r="G232" s="91"/>
     </row>
     <row r="233" spans="1:7">
       <c r="A233" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B233" s="89" t="s">
+      <c r="B233" s="92" t="s">
         <v>77</v>
       </c>
-      <c r="C233" s="90"/>
-      <c r="D233" s="90"/>
-      <c r="E233" s="91"/>
+      <c r="C233" s="93"/>
+      <c r="D233" s="93"/>
+      <c r="E233" s="94"/>
       <c r="F233" s="51" t="s">
         <v>46</v>
       </c>
@@ -10014,14 +10109,14 @@
       <c r="A234" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B234" s="92" t="s">
+      <c r="B234" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C234" s="93"/>
-      <c r="D234" s="93"/>
-      <c r="E234" s="93"/>
-      <c r="F234" s="93"/>
-      <c r="G234" s="94"/>
+      <c r="C234" s="96"/>
+      <c r="D234" s="96"/>
+      <c r="E234" s="96"/>
+      <c r="F234" s="96"/>
+      <c r="G234" s="97"/>
     </row>
     <row r="235" spans="1:7">
       <c r="A235" s="54" t="s">
@@ -10152,23 +10247,23 @@
       <c r="A242" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B242" s="95"/>
-      <c r="C242" s="96"/>
-      <c r="D242" s="96"/>
-      <c r="E242" s="96"/>
-      <c r="F242" s="96"/>
-      <c r="G242" s="97"/>
+      <c r="B242" s="89"/>
+      <c r="C242" s="90"/>
+      <c r="D242" s="90"/>
+      <c r="E242" s="90"/>
+      <c r="F242" s="90"/>
+      <c r="G242" s="91"/>
     </row>
     <row r="243" spans="1:7">
       <c r="A243" s="50" t="s">
         <v>228</v>
       </c>
-      <c r="B243" s="89" t="s">
+      <c r="B243" s="92" t="s">
         <v>79</v>
       </c>
-      <c r="C243" s="90"/>
-      <c r="D243" s="90"/>
-      <c r="E243" s="91"/>
+      <c r="C243" s="93"/>
+      <c r="D243" s="93"/>
+      <c r="E243" s="94"/>
       <c r="F243" s="51" t="s">
         <v>46</v>
       </c>
@@ -10181,14 +10276,14 @@
       <c r="A244" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B244" s="92" t="s">
+      <c r="B244" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C244" s="93"/>
-      <c r="D244" s="93"/>
-      <c r="E244" s="93"/>
-      <c r="F244" s="93"/>
-      <c r="G244" s="94"/>
+      <c r="C244" s="96"/>
+      <c r="D244" s="96"/>
+      <c r="E244" s="96"/>
+      <c r="F244" s="96"/>
+      <c r="G244" s="97"/>
     </row>
     <row r="245" spans="1:7">
       <c r="A245" s="54" t="s">
@@ -10302,23 +10397,23 @@
       <c r="A251" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B251" s="95"/>
-      <c r="C251" s="96"/>
-      <c r="D251" s="96"/>
-      <c r="E251" s="96"/>
-      <c r="F251" s="96"/>
-      <c r="G251" s="97"/>
+      <c r="B251" s="89"/>
+      <c r="C251" s="90"/>
+      <c r="D251" s="90"/>
+      <c r="E251" s="90"/>
+      <c r="F251" s="90"/>
+      <c r="G251" s="91"/>
     </row>
     <row r="252" spans="1:7">
       <c r="A252" s="50" t="s">
         <v>240</v>
       </c>
-      <c r="B252" s="89" t="s">
+      <c r="B252" s="92" t="s">
         <v>241</v>
       </c>
-      <c r="C252" s="90"/>
-      <c r="D252" s="90"/>
-      <c r="E252" s="91"/>
+      <c r="C252" s="93"/>
+      <c r="D252" s="93"/>
+      <c r="E252" s="94"/>
       <c r="F252" s="51" t="s">
         <v>46</v>
       </c>
@@ -10331,14 +10426,14 @@
       <c r="A253" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B253" s="92" t="s">
+      <c r="B253" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C253" s="93"/>
-      <c r="D253" s="93"/>
-      <c r="E253" s="93"/>
-      <c r="F253" s="93"/>
-      <c r="G253" s="94"/>
+      <c r="C253" s="96"/>
+      <c r="D253" s="96"/>
+      <c r="E253" s="96"/>
+      <c r="F253" s="96"/>
+      <c r="G253" s="97"/>
     </row>
     <row r="254" spans="1:7">
       <c r="A254" s="54" t="s">
@@ -10435,23 +10530,23 @@
       <c r="A259" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B259" s="95"/>
-      <c r="C259" s="96"/>
-      <c r="D259" s="96"/>
-      <c r="E259" s="96"/>
-      <c r="F259" s="96"/>
-      <c r="G259" s="97"/>
+      <c r="B259" s="89"/>
+      <c r="C259" s="90"/>
+      <c r="D259" s="90"/>
+      <c r="E259" s="90"/>
+      <c r="F259" s="90"/>
+      <c r="G259" s="91"/>
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="50" t="s">
         <v>260</v>
       </c>
-      <c r="B260" s="89" t="s">
+      <c r="B260" s="92" t="s">
         <v>258</v>
       </c>
-      <c r="C260" s="90"/>
-      <c r="D260" s="90"/>
-      <c r="E260" s="91"/>
+      <c r="C260" s="93"/>
+      <c r="D260" s="93"/>
+      <c r="E260" s="94"/>
       <c r="F260" s="51" t="s">
         <v>46</v>
       </c>
@@ -10464,14 +10559,14 @@
       <c r="A261" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B261" s="92" t="s">
+      <c r="B261" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="C261" s="93"/>
-      <c r="D261" s="93"/>
-      <c r="E261" s="93"/>
-      <c r="F261" s="93"/>
-      <c r="G261" s="94"/>
+      <c r="C261" s="96"/>
+      <c r="D261" s="96"/>
+      <c r="E261" s="96"/>
+      <c r="F261" s="96"/>
+      <c r="G261" s="97"/>
     </row>
     <row r="262" spans="1:7">
       <c r="A262" s="54" t="s">
@@ -10589,237 +10684,434 @@
       <c r="A268" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B268" s="95"/>
-      <c r="C268" s="96"/>
-      <c r="D268" s="96"/>
-      <c r="E268" s="96"/>
-      <c r="F268" s="96"/>
-      <c r="G268" s="97"/>
-    </row>
-    <row r="269" spans="1:7">
-      <c r="A269"/>
-      <c r="B269"/>
-      <c r="C269"/>
-      <c r="D269"/>
-      <c r="E269"/>
-      <c r="F269"/>
-      <c r="G269"/>
-    </row>
-    <row r="270" spans="1:7">
-      <c r="A270"/>
-      <c r="B270"/>
-      <c r="C270"/>
-      <c r="D270"/>
-      <c r="E270"/>
-      <c r="F270"/>
-      <c r="G270"/>
-    </row>
-    <row r="271" spans="1:7">
-      <c r="A271"/>
-      <c r="B271"/>
-      <c r="C271"/>
-      <c r="D271"/>
-      <c r="E271"/>
-      <c r="F271"/>
-      <c r="G271"/>
-    </row>
-    <row r="272" spans="1:7">
-      <c r="A272"/>
-      <c r="B272"/>
-      <c r="C272"/>
-      <c r="D272"/>
-      <c r="E272"/>
-      <c r="F272"/>
-      <c r="G272"/>
-    </row>
-    <row r="273" spans="1:7">
-      <c r="A273"/>
-      <c r="B273"/>
-      <c r="C273"/>
-      <c r="D273"/>
-      <c r="E273"/>
-      <c r="F273"/>
-      <c r="G273"/>
-    </row>
-    <row r="274" spans="1:7">
-      <c r="A274"/>
-      <c r="B274"/>
-      <c r="C274"/>
-      <c r="D274"/>
-      <c r="E274"/>
-      <c r="F274"/>
-      <c r="G274"/>
-    </row>
-    <row r="275" spans="1:7">
-      <c r="A275"/>
-      <c r="B275"/>
-      <c r="C275"/>
-      <c r="D275"/>
-      <c r="E275"/>
-      <c r="F275"/>
-      <c r="G275"/>
-    </row>
-    <row r="276" spans="1:7">
-      <c r="A276"/>
-      <c r="B276"/>
-      <c r="C276"/>
-      <c r="D276"/>
-      <c r="E276"/>
-      <c r="F276"/>
-      <c r="G276"/>
-    </row>
-    <row r="277" spans="1:7">
-      <c r="A277"/>
-      <c r="B277"/>
-      <c r="C277"/>
-      <c r="D277"/>
-      <c r="E277"/>
-      <c r="F277"/>
-      <c r="G277"/>
-    </row>
-    <row r="278" spans="1:7">
-      <c r="A278"/>
-      <c r="B278"/>
-      <c r="C278"/>
-      <c r="D278"/>
-      <c r="E278"/>
-      <c r="F278"/>
-      <c r="G278"/>
-    </row>
-    <row r="279" spans="1:7">
-      <c r="A279"/>
-      <c r="B279"/>
-      <c r="C279"/>
-      <c r="D279"/>
-      <c r="E279"/>
-      <c r="F279"/>
-      <c r="G279"/>
-    </row>
-    <row r="280" spans="1:7">
-      <c r="A280"/>
-      <c r="B280"/>
-      <c r="C280"/>
-      <c r="D280"/>
-      <c r="E280"/>
-      <c r="F280"/>
-      <c r="G280"/>
-    </row>
-    <row r="281" spans="1:7">
-      <c r="A281"/>
-      <c r="B281"/>
-      <c r="C281"/>
-      <c r="D281"/>
-      <c r="E281"/>
-      <c r="F281"/>
-      <c r="G281"/>
-    </row>
-    <row r="282" spans="1:7">
-      <c r="A282"/>
-      <c r="B282"/>
-      <c r="C282"/>
-      <c r="D282"/>
-      <c r="E282"/>
-      <c r="F282"/>
-      <c r="G282"/>
-    </row>
-    <row r="283" spans="1:7">
-      <c r="A283"/>
-      <c r="B283"/>
-      <c r="C283"/>
-      <c r="D283"/>
-      <c r="E283"/>
-      <c r="F283"/>
-      <c r="G283"/>
-    </row>
-    <row r="284" spans="1:7">
-      <c r="A284"/>
-      <c r="B284"/>
-      <c r="C284"/>
-      <c r="D284"/>
-      <c r="E284"/>
-      <c r="F284"/>
-      <c r="G284"/>
-    </row>
-    <row r="285" spans="1:7">
-      <c r="A285"/>
-      <c r="B285"/>
-      <c r="C285"/>
-      <c r="D285"/>
-      <c r="E285"/>
-      <c r="F285"/>
-      <c r="G285"/>
-    </row>
-    <row r="286" spans="1:7">
-      <c r="A286"/>
-      <c r="B286"/>
-      <c r="C286"/>
-      <c r="D286"/>
-      <c r="E286"/>
-      <c r="F286"/>
-      <c r="G286"/>
-    </row>
-    <row r="287" spans="1:7">
-      <c r="A287"/>
-      <c r="B287"/>
-      <c r="C287"/>
-      <c r="D287"/>
-      <c r="E287"/>
-      <c r="F287"/>
-      <c r="G287"/>
-    </row>
-    <row r="288" spans="1:7">
-      <c r="A288"/>
-      <c r="B288"/>
-      <c r="C288"/>
-      <c r="D288"/>
-      <c r="E288"/>
-      <c r="F288"/>
-      <c r="G288"/>
-    </row>
-    <row r="289" spans="1:7">
-      <c r="A289"/>
-      <c r="B289"/>
-      <c r="C289"/>
-      <c r="D289"/>
-      <c r="E289"/>
-      <c r="F289"/>
-      <c r="G289"/>
-    </row>
-    <row r="290" spans="1:7">
-      <c r="A290"/>
-      <c r="B290"/>
-      <c r="C290"/>
-      <c r="D290"/>
-      <c r="E290"/>
-      <c r="F290"/>
-      <c r="G290"/>
-    </row>
-    <row r="291" spans="1:7">
-      <c r="A291"/>
-      <c r="B291"/>
-      <c r="C291"/>
-      <c r="D291"/>
-      <c r="E291"/>
-      <c r="F291"/>
-      <c r="G291"/>
-    </row>
-    <row r="292" spans="1:7">
-      <c r="A292"/>
-      <c r="B292"/>
-      <c r="C292"/>
-      <c r="D292"/>
-      <c r="E292"/>
-      <c r="F292"/>
-      <c r="G292"/>
-    </row>
-    <row r="293" spans="1:7">
-      <c r="A293"/>
-      <c r="B293"/>
-      <c r="C293"/>
-      <c r="D293"/>
-      <c r="E293"/>
-      <c r="F293"/>
-      <c r="G293"/>
+      <c r="B268" s="89"/>
+      <c r="C268" s="90"/>
+      <c r="D268" s="90"/>
+      <c r="E268" s="90"/>
+      <c r="F268" s="90"/>
+      <c r="G268" s="91"/>
+    </row>
+    <row r="269" spans="1:7" customFormat="1">
+      <c r="A269" s="50" t="s">
+        <v>268</v>
+      </c>
+      <c r="B269" s="92" t="s">
+        <v>269</v>
+      </c>
+      <c r="C269" s="93"/>
+      <c r="D269" s="93"/>
+      <c r="E269" s="94"/>
+      <c r="F269" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="G269" s="52" t="str">
+        <f>IF(COUNTIF(F272:F274,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F272:F274,"Fail")&gt;0,"Fail",IF(COUNTIF(F272:F274,"")=0,"Pass","Not Executed")))</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="270" spans="1:7" customFormat="1">
+      <c r="A270" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B270" s="95" t="s">
+        <v>48</v>
+      </c>
+      <c r="C270" s="96"/>
+      <c r="D270" s="96"/>
+      <c r="E270" s="96"/>
+      <c r="F270" s="96"/>
+      <c r="G270" s="97"/>
+    </row>
+    <row r="271" spans="1:7" customFormat="1">
+      <c r="A271" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B271" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C271" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D271" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E271" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F271" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G271" s="54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="272" spans="1:7" customFormat="1" ht="149.25" customHeight="1">
+      <c r="A272" s="55">
+        <v>1</v>
+      </c>
+      <c r="B272" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C272" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="D272" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="E272" s="57"/>
+      <c r="F272" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G272" s="59"/>
+    </row>
+    <row r="273" spans="1:7" customFormat="1" ht="81" customHeight="1">
+      <c r="A273" s="55">
+        <v>2</v>
+      </c>
+      <c r="B273" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="C273" s="57" t="s">
+        <v>273</v>
+      </c>
+      <c r="D273" s="57"/>
+      <c r="E273" s="57"/>
+      <c r="F273" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G273" s="59"/>
+    </row>
+    <row r="274" spans="1:7" customFormat="1" ht="38.25" customHeight="1">
+      <c r="A274" s="55">
+        <v>3</v>
+      </c>
+      <c r="B274" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="C274" s="57" t="s">
+        <v>275</v>
+      </c>
+      <c r="D274" s="57"/>
+      <c r="E274" s="57"/>
+      <c r="F274" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G274" s="59"/>
+    </row>
+    <row r="275" spans="1:7" customFormat="1" ht="63.75" customHeight="1">
+      <c r="A275" s="55">
+        <v>4</v>
+      </c>
+      <c r="B275" s="56" t="s">
+        <v>276</v>
+      </c>
+      <c r="C275" s="57" t="s">
+        <v>277</v>
+      </c>
+      <c r="D275" s="57"/>
+      <c r="E275" s="57"/>
+      <c r="F275" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G275" s="59"/>
+    </row>
+    <row r="276" spans="1:7" customFormat="1">
+      <c r="A276" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B276" s="89"/>
+      <c r="C276" s="90"/>
+      <c r="D276" s="90"/>
+      <c r="E276" s="90"/>
+      <c r="F276" s="90"/>
+      <c r="G276" s="91"/>
+    </row>
+    <row r="277" spans="1:7" customFormat="1">
+      <c r="A277" s="50" t="s">
+        <v>278</v>
+      </c>
+      <c r="B277" s="92" t="s">
+        <v>279</v>
+      </c>
+      <c r="C277" s="93"/>
+      <c r="D277" s="93"/>
+      <c r="E277" s="94"/>
+      <c r="F277" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="G277" s="52" t="str">
+        <f>IF(COUNTIF(F280:F282,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F280:F282,"Fail")&gt;0,"Fail",IF(COUNTIF(F280:F282,"")=0,"Pass","Not Executed")))</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="278" spans="1:7" customFormat="1">
+      <c r="A278" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B278" s="95" t="s">
+        <v>48</v>
+      </c>
+      <c r="C278" s="96"/>
+      <c r="D278" s="96"/>
+      <c r="E278" s="96"/>
+      <c r="F278" s="96"/>
+      <c r="G278" s="97"/>
+    </row>
+    <row r="279" spans="1:7" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A279" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B279" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C279" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D279" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E279" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F279" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G279" s="54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="280" spans="1:7" customFormat="1" ht="162" customHeight="1">
+      <c r="A280" s="55">
+        <v>1</v>
+      </c>
+      <c r="B280" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C280" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="D280" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="E280" s="57"/>
+      <c r="F280" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G280" s="59"/>
+    </row>
+    <row r="281" spans="1:7" customFormat="1" ht="42" customHeight="1">
+      <c r="A281" s="55">
+        <v>2</v>
+      </c>
+      <c r="B281" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="C281" s="57" t="s">
+        <v>273</v>
+      </c>
+      <c r="D281" s="57"/>
+      <c r="E281" s="57"/>
+      <c r="F281" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G281" s="59"/>
+    </row>
+    <row r="282" spans="1:7" customFormat="1" ht="56.25" customHeight="1">
+      <c r="A282" s="55">
+        <v>3</v>
+      </c>
+      <c r="B282" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="C282" s="57" t="s">
+        <v>281</v>
+      </c>
+      <c r="D282" s="57"/>
+      <c r="E282" s="57"/>
+      <c r="F282" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G282" s="59"/>
+    </row>
+    <row r="283" spans="1:7" customFormat="1" ht="61.5" customHeight="1">
+      <c r="A283" s="55">
+        <v>4</v>
+      </c>
+      <c r="B283" s="56" t="s">
+        <v>274</v>
+      </c>
+      <c r="C283" s="57" t="s">
+        <v>282</v>
+      </c>
+      <c r="D283" s="57"/>
+      <c r="E283" s="57"/>
+      <c r="F283" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G283" s="59"/>
+    </row>
+    <row r="284" spans="1:7" customFormat="1" ht="56.25" customHeight="1">
+      <c r="A284" s="55">
+        <v>5</v>
+      </c>
+      <c r="B284" s="56" t="s">
+        <v>283</v>
+      </c>
+      <c r="C284" s="57" t="s">
+        <v>284</v>
+      </c>
+      <c r="D284" s="57"/>
+      <c r="E284" s="57"/>
+      <c r="F284" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G284" s="59"/>
+    </row>
+    <row r="285" spans="1:7" customFormat="1">
+      <c r="A285" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B285" s="89"/>
+      <c r="C285" s="90"/>
+      <c r="D285" s="90"/>
+      <c r="E285" s="90"/>
+      <c r="F285" s="90"/>
+      <c r="G285" s="91"/>
+    </row>
+    <row r="286" spans="1:7" customFormat="1">
+      <c r="A286" s="50" t="s">
+        <v>285</v>
+      </c>
+      <c r="B286" s="92" t="s">
+        <v>286</v>
+      </c>
+      <c r="C286" s="93"/>
+      <c r="D286" s="93"/>
+      <c r="E286" s="94"/>
+      <c r="F286" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="G286" s="52" t="str">
+        <f>IF(COUNTIF(F289:F291,"Blocked")&gt;0,"Blocked",IF(COUNTIF(F289:F291,"Fail")&gt;0,"Fail",IF(COUNTIF(F289:F291,"")=0,"Pass","Not Executed")))</f>
+        <v>Pass</v>
+      </c>
+    </row>
+    <row r="287" spans="1:7" customFormat="1">
+      <c r="A287" s="53" t="s">
+        <v>47</v>
+      </c>
+      <c r="B287" s="95" t="s">
+        <v>48</v>
+      </c>
+      <c r="C287" s="96"/>
+      <c r="D287" s="96"/>
+      <c r="E287" s="96"/>
+      <c r="F287" s="96"/>
+      <c r="G287" s="97"/>
+    </row>
+    <row r="288" spans="1:7" customFormat="1">
+      <c r="A288" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="B288" s="54" t="s">
+        <v>50</v>
+      </c>
+      <c r="C288" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="D288" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="E288" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="F288" s="54" t="s">
+        <v>54</v>
+      </c>
+      <c r="G288" s="54" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" customFormat="1" ht="135">
+      <c r="A289" s="55">
+        <v>1</v>
+      </c>
+      <c r="B289" s="56" t="s">
+        <v>56</v>
+      </c>
+      <c r="C289" s="57" t="s">
+        <v>270</v>
+      </c>
+      <c r="D289" s="57" t="s">
+        <v>271</v>
+      </c>
+      <c r="E289" s="57"/>
+      <c r="F289" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G289" s="59"/>
+    </row>
+    <row r="290" spans="1:7" customFormat="1" ht="45">
+      <c r="A290" s="55">
+        <v>2</v>
+      </c>
+      <c r="B290" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="C290" s="57" t="s">
+        <v>287</v>
+      </c>
+      <c r="D290" s="57"/>
+      <c r="E290" s="57"/>
+      <c r="F290" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G290" s="59"/>
+    </row>
+    <row r="291" spans="1:7" customFormat="1" ht="45">
+      <c r="A291" s="55">
+        <v>3</v>
+      </c>
+      <c r="B291" s="56" t="s">
+        <v>288</v>
+      </c>
+      <c r="C291" s="57" t="s">
+        <v>289</v>
+      </c>
+      <c r="D291" s="57"/>
+      <c r="E291" s="57"/>
+      <c r="F291" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G291" s="59"/>
+    </row>
+    <row r="292" spans="1:7" s="104" customFormat="1" ht="91.5" customHeight="1">
+      <c r="A292" s="55">
+        <v>4</v>
+      </c>
+      <c r="B292" s="56" t="s">
+        <v>290</v>
+      </c>
+      <c r="C292" s="57" t="s">
+        <v>291</v>
+      </c>
+      <c r="D292" s="57"/>
+      <c r="E292" s="57"/>
+      <c r="F292" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="G292" s="59"/>
+    </row>
+    <row r="293" spans="1:7" customFormat="1">
+      <c r="A293" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="B293" s="89"/>
+      <c r="C293" s="90"/>
+      <c r="D293" s="90"/>
+      <c r="E293" s="90"/>
+      <c r="F293" s="90"/>
+      <c r="G293" s="91"/>
     </row>
     <row r="294" spans="1:7">
       <c r="A294"/>
@@ -16822,64 +17114,16 @@
       <c r="H960" s="25"/>
     </row>
   </sheetData>
-  <mergeCells count="73">
-    <mergeCell ref="B259:G259"/>
-    <mergeCell ref="B243:E243"/>
-    <mergeCell ref="B244:G244"/>
-    <mergeCell ref="B251:G251"/>
-    <mergeCell ref="B252:E252"/>
-    <mergeCell ref="B253:G253"/>
-    <mergeCell ref="B221:G221"/>
-    <mergeCell ref="B232:G232"/>
-    <mergeCell ref="B233:E233"/>
-    <mergeCell ref="B234:G234"/>
-    <mergeCell ref="B242:G242"/>
-    <mergeCell ref="B209:G209"/>
-    <mergeCell ref="B210:E210"/>
-    <mergeCell ref="B211:G211"/>
-    <mergeCell ref="B219:G219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B176:E176"/>
-    <mergeCell ref="B177:G177"/>
-    <mergeCell ref="B190:G190"/>
-    <mergeCell ref="B191:E191"/>
-    <mergeCell ref="B192:G192"/>
-    <mergeCell ref="B148:G148"/>
-    <mergeCell ref="B161:G161"/>
-    <mergeCell ref="B162:E162"/>
-    <mergeCell ref="B163:G163"/>
-    <mergeCell ref="B175:G175"/>
-    <mergeCell ref="B132:G132"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="B134:G134"/>
-    <mergeCell ref="B146:G146"/>
-    <mergeCell ref="B147:E147"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B72:G72"/>
+  <mergeCells count="82">
+    <mergeCell ref="B285:G285"/>
+    <mergeCell ref="B286:E286"/>
+    <mergeCell ref="B287:G287"/>
+    <mergeCell ref="B293:G293"/>
+    <mergeCell ref="B269:E269"/>
+    <mergeCell ref="B270:G270"/>
+    <mergeCell ref="B276:G276"/>
+    <mergeCell ref="B277:E277"/>
+    <mergeCell ref="B278:G278"/>
     <mergeCell ref="B260:E260"/>
     <mergeCell ref="B261:G261"/>
     <mergeCell ref="B268:G268"/>
@@ -16896,9 +17140,66 @@
     <mergeCell ref="B118:G118"/>
     <mergeCell ref="B119:E119"/>
     <mergeCell ref="B120:G120"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B72:G72"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B132:G132"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="B134:G134"/>
+    <mergeCell ref="B146:G146"/>
+    <mergeCell ref="B147:E147"/>
+    <mergeCell ref="B148:G148"/>
+    <mergeCell ref="B161:G161"/>
+    <mergeCell ref="B162:E162"/>
+    <mergeCell ref="B163:G163"/>
+    <mergeCell ref="B175:G175"/>
+    <mergeCell ref="B176:E176"/>
+    <mergeCell ref="B177:G177"/>
+    <mergeCell ref="B190:G190"/>
+    <mergeCell ref="B191:E191"/>
+    <mergeCell ref="B192:G192"/>
+    <mergeCell ref="B209:G209"/>
+    <mergeCell ref="B210:E210"/>
+    <mergeCell ref="B211:G211"/>
+    <mergeCell ref="B219:G219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B221:G221"/>
+    <mergeCell ref="B232:G232"/>
+    <mergeCell ref="B233:E233"/>
+    <mergeCell ref="B234:G234"/>
+    <mergeCell ref="B242:G242"/>
+    <mergeCell ref="B259:G259"/>
+    <mergeCell ref="B243:E243"/>
+    <mergeCell ref="B244:G244"/>
+    <mergeCell ref="B251:G251"/>
+    <mergeCell ref="B252:E252"/>
+    <mergeCell ref="B253:G253"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F443:F445 F450:F456 F669:F671 F659:F664 F461:F470 F475:F478 F483:F488 F493:F501 F506:F515 F520:F530 F535:F545 F561:F567 F589:F591 F550:F556 F572:F578 F583:F584 F596:F602 F607:F613 F629:F631 F618:F624 F636:F639 F644:F646 F651:F654 F21:F22 F50:F53 F34:F37 F27:F29 F82:F90 F42:F45 F66:F69 F74:F77 F58:F61 F95:F104 F109:F117 F122:F131 F136:F145 F150:F160 F165:F174 F179:F189 F194:F208 F213:F218 F223:F231 F236:F241 F246:F250 F255:F258 F263:F267">
+    <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F443:F445 F450:F456 F669:F671 F659:F664 F461:F470 F475:F478 F483:F488 F493:F501 F506:F515 F520:F530 F535:F545 F561:F567 F589:F591 F550:F556 F572:F578 F583:F584 F596:F602 F607:F613 F629:F631 F618:F624 F636:F639 F644:F646 F651:F654 F21:F22 F50:F53 F34:F37 F27:F29 F82:F90 F42:F45 F66:F69 F74:F77 F58:F61 F95:F104 F109:F117 F122:F131 F136:F145 F150:F160 F165:F174 F179:F189 F194:F208 F213:F218 F223:F231 F236:F241 F246:F250 F255:F258 F263:F267 F272:F275 F280:F284 F289:F292">
       <formula1>"Pass, Fail, Blocked"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Carousel formatting of last 3 cases
</commit_message>
<xml_diff>
--- a/TCS_NEWUI_Carousel.xlsx
+++ b/TCS_NEWUI_Carousel.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" tabRatio="815" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="12240" tabRatio="815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="5" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="296">
   <si>
     <t>Test Case Result Modules-Wise</t>
   </si>
@@ -904,9 +904,6 @@
 2. Sorted by option should be removed from carousel</t>
   </si>
   <si>
-    <t>US:WEB-7848_TC 01</t>
-  </si>
-  <si>
     <t>Verify Carousel  when the default selected sorting option is First Run date</t>
   </si>
   <si>
@@ -943,9 +940,6 @@
     <t>User should be able to see that all the Ads in the Carousel are sorted in Descending order as per their First Run Date</t>
   </si>
   <si>
-    <t>US:WEB-7848_TC 02</t>
-  </si>
-  <si>
     <t>Verify Carousel When user selects sorting option SPEND</t>
   </si>
   <si>
@@ -962,9 +956,6 @@
   </si>
   <si>
     <t>User should be able to see that all the Ads in the Carousel are sorted in Descending order as per their Spend data</t>
-  </si>
-  <si>
-    <t>US:WEB-7848_TC 03</t>
   </si>
   <si>
     <t>Verify the Carousel Ad tiles field by switching the sorting options</t>
@@ -989,6 +980,27 @@
     <t>1.User should be able to switch to First Run Date option for sorting of Carousel 
 2. Ads in the carousel should show the media and First Run Date data on it
 3. Ads should be sorted in descending order as per their First Run Date</t>
+  </si>
+  <si>
+    <t>TC24</t>
+  </si>
+  <si>
+    <t>TC25</t>
+  </si>
+  <si>
+    <t>TC26</t>
+  </si>
+  <si>
+    <t>US:WEB-7428_TC 24</t>
+  </si>
+  <si>
+    <t>US:WEB-7428_TC 25</t>
+  </si>
+  <si>
+    <t>US:WEB-7428_TC 26</t>
+  </si>
+  <si>
+    <t>SMRT-7987</t>
   </si>
 </sst>
 </file>
@@ -2682,14 +2694,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="152" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="31" borderId="42" xfId="144" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="35" fillId="21" borderId="1" xfId="134" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2762,7 +2770,15 @@
     <xf numFmtId="0" fontId="50" fillId="29" borderId="39" xfId="144" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="152" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="156">
     <cellStyle name="20% - Accent1" xfId="11"/>
@@ -3043,7 +3059,7 @@
           <c:x val="5.3923741222529187E-2"/>
           <c:y val="0.14185650994577867"/>
           <c:w val="0.90694002510216154"/>
-          <c:h val="0.75521895211321854"/>
+          <c:h val="0.75521895211321866"/>
         </c:manualLayout>
       </c:layout>
       <c:barChart>
@@ -3225,11 +3241,11 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:axId val="73763456"/>
-        <c:axId val="73773440"/>
+        <c:axId val="72632960"/>
+        <c:axId val="72642944"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="73763456"/>
+        <c:axId val="72632960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3248,14 +3264,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73773440"/>
+        <c:crossAx val="72642944"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="73773440"/>
+        <c:axId val="72642944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3263,7 +3279,7 @@
         <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="73763456"/>
+        <c:crossAx val="72632960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3283,7 +3299,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000533" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000533" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000544" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000544" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3329,8 +3345,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="3.8831278392536694E-2"/>
-          <c:y val="0.14624350369603392"/>
-          <c:w val="0.92496729254319754"/>
+          <c:y val="0.14624350369603395"/>
+          <c:w val="0.92496729254319776"/>
           <c:h val="0.69766331701963369"/>
         </c:manualLayout>
       </c:layout>
@@ -3474,8 +3490,8 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.270891046791853"/>
-          <c:y val="0.88141746683253475"/>
-          <c:w val="0.4279103679659812"/>
+          <c:y val="0.88141746683253452"/>
+          <c:w val="0.42791036796598136"/>
           <c:h val="7.1280252974084315E-2"/>
         </c:manualLayout>
       </c:layout>
@@ -3495,7 +3511,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000377" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000377" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000389" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000389" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -3513,9 +3529,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.27595722641494741"/>
-          <c:y val="7.1365887012686396E-2"/>
-          <c:w val="0.2967237552279261"/>
-          <c:h val="0.85466509216403863"/>
+          <c:y val="7.136588701268641E-2"/>
+          <c:w val="0.29672375522792616"/>
+          <c:h val="0.85466509216403874"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -3719,8 +3735,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.72165251246917483"/>
-          <c:y val="3.6083951617898596E-3"/>
+          <c:x val="0.72165251246917506"/>
+          <c:y val="3.6083951617898601E-3"/>
           <c:w val="0.24112408909611374"/>
           <c:h val="0.95693837006674254"/>
         </c:manualLayout>
@@ -3782,7 +3798,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter alignWithMargins="0"/>
-    <c:pageMargins b="1" l="0.75000000000000033" r="0.75000000000000033" t="1" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75000000000000044" r="0.75000000000000044" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3808,7 +3824,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3846,7 +3862,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3884,7 +3900,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{AB276036-E4AE-4D63-9C65-0694CB3986A9}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB276036-E4AE-4D63-9C65-0694CB3986A9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3896,7 +3912,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -3916,7 +3932,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -3988,7 +4004,7 @@
           <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5AF65C03-9B72-4D6B-9DD9-6AFF172BC3B5}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AF65C03-9B72-4D6B-9DD9-6AFF172BC3B5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4122,7 +4138,7 @@
         </a:effectLst>
         <a:extLst>
           <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" w="9525" cmpd="sng">
+            <a14:hiddenLine xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525" cmpd="sng">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -4172,7 +4188,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{E67F1DD6-8FFA-4013-AC77-D7090A499C80}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E67F1DD6-8FFA-4013-AC77-D7090A499C80}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4541,33 +4557,33 @@
   </cols>
   <sheetData>
     <row r="5" spans="1:7" ht="18" customHeight="1">
-      <c r="A5" s="80" t="s">
+      <c r="A5" s="78" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
+      <c r="B5" s="79"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
     </row>
     <row r="6" spans="1:7" ht="18" customHeight="1">
-      <c r="A6" s="82" t="s">
+      <c r="A6" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="82" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="85"/>
-      <c r="D6" s="85"/>
-      <c r="E6" s="85"/>
-      <c r="F6" s="86"/>
-      <c r="G6" s="87" t="s">
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
+      <c r="E6" s="83"/>
+      <c r="F6" s="84"/>
+      <c r="G6" s="85" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="30.75" thickBot="1">
-      <c r="A7" s="83"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="10" t="s">
         <v>4</v>
       </c>
@@ -4583,7 +4599,7 @@
       <c r="F7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="87"/>
+      <c r="G7" s="85"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" thickTop="1">
       <c r="A8" s="1" t="s">
@@ -4684,15 +4700,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G103"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36.5703125" style="3" customWidth="1"/>
     <col min="2" max="2" width="18.5703125" style="8" customWidth="1"/>
-    <col min="3" max="3" width="115.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="69.28515625" style="3" customWidth="1"/>
     <col min="5" max="256" width="9" style="3"/>
     <col min="257" max="257" width="71.85546875" style="3" customWidth="1"/>
@@ -4961,7 +4977,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" ht="16.5" customHeight="1">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="86" t="s">
         <v>65</v>
       </c>
       <c r="B2" s="70" t="s">
@@ -4974,74 +4990,74 @@
       <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="88"/>
+      <c r="A3" s="86"/>
       <c r="B3" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="68" t="s">
+      <c r="C3" s="71" t="s">
         <v>67</v>
       </c>
       <c r="D3" s="68"/>
       <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" s="20" customFormat="1">
-      <c r="A4" s="88"/>
+      <c r="A4" s="86"/>
       <c r="B4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="21" t="s">
         <v>72</v>
       </c>
       <c r="D4" s="68"/>
       <c r="E4" s="21"/>
     </row>
     <row r="5" spans="1:5" s="22" customFormat="1">
-      <c r="A5" s="88"/>
+      <c r="A5" s="86"/>
       <c r="B5" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="21" t="s">
         <v>71</v>
       </c>
       <c r="D5" s="68"/>
       <c r="E5" s="23"/>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="88"/>
+      <c r="A6" s="86"/>
       <c r="B6" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="20" t="s">
+      <c r="C6" s="21" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="5"/>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="88"/>
+      <c r="A7" s="86"/>
       <c r="B7" s="67" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="21" t="s">
         <v>69</v>
       </c>
       <c r="E7" s="5"/>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="88"/>
+      <c r="A8" s="86"/>
       <c r="B8" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="21" t="s">
         <v>70</v>
       </c>
       <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="88"/>
+      <c r="A9" s="86"/>
       <c r="B9" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="76" t="s">
+      <c r="C9" s="102" t="s">
         <v>92</v>
       </c>
       <c r="D9" s="71" t="s">
@@ -5050,11 +5066,11 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:5" ht="45">
-      <c r="A10" s="88"/>
+      <c r="A10" s="86"/>
       <c r="B10" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="72" t="s">
         <v>80</v>
       </c>
       <c r="D10" s="72" t="s">
@@ -5062,28 +5078,28 @@
       </c>
       <c r="E10" s="5"/>
     </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="88"/>
+    <row r="11" spans="1:5" ht="30">
+      <c r="A11" s="86"/>
       <c r="B11" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="68" t="s">
+      <c r="C11" s="71" t="s">
         <v>90</v>
       </c>
       <c r="E11" s="5"/>
     </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="88"/>
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="86"/>
       <c r="B12" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="103" t="s">
         <v>89</v>
       </c>
       <c r="E12" s="5"/>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="88"/>
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" s="86"/>
       <c r="B13" s="19" t="s">
         <v>22</v>
       </c>
@@ -5092,18 +5108,18 @@
       </c>
       <c r="E13" s="5"/>
     </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="88"/>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="86"/>
       <c r="B14" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="77" t="s">
+      <c r="C14" s="103" t="s">
         <v>87</v>
       </c>
       <c r="E14" s="5"/>
     </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="88"/>
+    <row r="15" spans="1:5" ht="30">
+      <c r="A15" s="86"/>
       <c r="B15" s="19" t="s">
         <v>94</v>
       </c>
@@ -5112,18 +5128,18 @@
       </c>
       <c r="E15" s="5"/>
     </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="88"/>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="86"/>
       <c r="B16" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="77" t="s">
+      <c r="C16" s="103" t="s">
         <v>85</v>
       </c>
       <c r="E16" s="5"/>
     </row>
-    <row r="17" spans="1:7">
-      <c r="A17" s="88"/>
+    <row r="17" spans="1:7" ht="30">
+      <c r="A17" s="86"/>
       <c r="B17" s="19" t="s">
         <v>96</v>
       </c>
@@ -5133,11 +5149,11 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:7">
-      <c r="A18" s="88"/>
+      <c r="A18" s="86"/>
       <c r="B18" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="78" t="s">
+      <c r="C18" s="104" t="s">
         <v>82</v>
       </c>
       <c r="D18" s="68" t="s">
@@ -5146,22 +5162,22 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="88"/>
+      <c r="A19" s="86"/>
       <c r="B19" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="78" t="s">
+      <c r="C19" s="104" t="s">
         <v>83</v>
       </c>
       <c r="D19" s="68"/>
       <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="88"/>
+      <c r="A20" s="86"/>
       <c r="B20" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="78" t="s">
+      <c r="C20" s="104" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="68" t="s">
@@ -5170,12 +5186,12 @@
       <c r="E20" s="5"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7">
-      <c r="A21" s="88"/>
+    <row r="21" spans="1:7" ht="30">
+      <c r="A21" s="86"/>
       <c r="B21" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="78" t="s">
+      <c r="C21" s="104" t="s">
         <v>77</v>
       </c>
       <c r="D21" s="68" t="s">
@@ -5185,11 +5201,11 @@
       <c r="G21"/>
     </row>
     <row r="22" spans="1:7">
-      <c r="A22" s="88"/>
+      <c r="A22" s="86"/>
       <c r="B22" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="78" t="s">
+      <c r="C22" s="104" t="s">
         <v>79</v>
       </c>
       <c r="D22" s="68" t="s">
@@ -5199,11 +5215,11 @@
       <c r="G22"/>
     </row>
     <row r="23" spans="1:7">
-      <c r="A23" s="88"/>
+      <c r="A23" s="86"/>
       <c r="B23" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="C23" s="72" t="s">
         <v>241</v>
       </c>
       <c r="D23" s="75"/>
@@ -5211,7 +5227,7 @@
       <c r="G23"/>
     </row>
     <row r="24" spans="1:7">
-      <c r="A24" s="88"/>
+      <c r="A24" s="86"/>
       <c r="B24" s="19" t="s">
         <v>257</v>
       </c>
@@ -5225,131 +5241,146 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="88"/>
-      <c r="B25" s="4"/>
-      <c r="D25" s="73"/>
+      <c r="A25" s="86"/>
+      <c r="B25" s="19" t="s">
+        <v>289</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>268</v>
+      </c>
+      <c r="D25" s="73" t="s">
+        <v>295</v>
+      </c>
       <c r="E25" s="5"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="88"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="73" t="s">
-        <v>91</v>
+      <c r="A26" s="86"/>
+      <c r="B26" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>277</v>
       </c>
       <c r="D26" s="68"/>
       <c r="E26" s="5"/>
       <c r="G26"/>
     </row>
     <row r="27" spans="1:7">
-      <c r="A27" s="88"/>
-      <c r="B27" s="4"/>
+      <c r="A27" s="86"/>
+      <c r="B27" s="19" t="s">
+        <v>291</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>283</v>
+      </c>
       <c r="D27" s="68"/>
       <c r="E27" s="5"/>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" s="88"/>
+      <c r="A28" s="86"/>
       <c r="B28" s="4"/>
       <c r="D28" s="68"/>
       <c r="E28" s="5"/>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" s="88"/>
+      <c r="A29" s="86"/>
       <c r="B29" s="4"/>
-      <c r="C29" s="68"/>
       <c r="D29" s="68"/>
       <c r="E29" s="5"/>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" s="88"/>
+      <c r="A30" s="86"/>
       <c r="B30" s="4"/>
       <c r="C30" s="68"/>
       <c r="D30" s="68"/>
       <c r="E30" s="5"/>
     </row>
     <row r="31" spans="1:7">
-      <c r="A31" s="88"/>
+      <c r="A31" s="86"/>
       <c r="B31" s="4"/>
-      <c r="C31" s="68"/>
+      <c r="C31" s="73" t="s">
+        <v>91</v>
+      </c>
       <c r="D31" s="68"/>
       <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" s="88"/>
+      <c r="A32" s="86"/>
       <c r="B32" s="4"/>
       <c r="C32" s="68"/>
       <c r="D32" s="68"/>
       <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5">
-      <c r="A33" s="88"/>
+      <c r="A33" s="86"/>
       <c r="B33" s="4"/>
       <c r="C33" s="68"/>
       <c r="D33" s="68"/>
       <c r="E33" s="5"/>
     </row>
     <row r="34" spans="1:5">
-      <c r="A34" s="88"/>
+      <c r="A34" s="86"/>
       <c r="B34" s="4"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5">
-      <c r="A35" s="88"/>
+      <c r="A35" s="86"/>
       <c r="B35" s="4"/>
       <c r="E35" s="5"/>
     </row>
     <row r="36" spans="1:5">
-      <c r="A36" s="88"/>
+      <c r="A36" s="86"/>
       <c r="B36" s="4"/>
       <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5">
-      <c r="A37" s="88"/>
+      <c r="A37" s="86"/>
       <c r="B37" s="4"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5">
-      <c r="A38" s="88"/>
+      <c r="A38" s="86"/>
       <c r="B38" s="4"/>
       <c r="E38" s="5"/>
     </row>
     <row r="39" spans="1:5">
-      <c r="A39" s="88"/>
+      <c r="A39" s="86"/>
       <c r="B39" s="4"/>
       <c r="C39" s="68"/>
       <c r="D39" s="68"/>
       <c r="E39" s="5"/>
     </row>
     <row r="40" spans="1:5">
-      <c r="A40" s="88"/>
+      <c r="A40" s="86"/>
       <c r="B40" s="4"/>
       <c r="C40" s="68"/>
       <c r="D40" s="68"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5">
-      <c r="A41" s="88"/>
+      <c r="A41" s="86"/>
       <c r="B41" s="4"/>
       <c r="D41" s="68"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5">
-      <c r="A42" s="88"/>
+      <c r="A42" s="86"/>
       <c r="B42" s="4"/>
       <c r="C42" s="6"/>
     </row>
     <row r="43" spans="1:5">
-      <c r="A43" s="88"/>
+      <c r="A43" s="86"/>
       <c r="B43" s="4"/>
       <c r="C43" s="6"/>
     </row>
     <row r="44" spans="1:5">
-      <c r="A44" s="88"/>
+      <c r="A44" s="86"/>
       <c r="B44" s="4"/>
       <c r="C44" s="6"/>
     </row>
     <row r="45" spans="1:5">
-      <c r="A45" s="88"/>
+      <c r="A45" s="86"/>
       <c r="B45" s="4"/>
       <c r="C45" s="6"/>
     </row>
@@ -5598,8 +5629,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A263" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B272" sqref="B272"/>
+    <sheetView topLeftCell="A269" zoomScale="90" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A269" sqref="A269"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15"/>
@@ -6265,10 +6296,10 @@
       </c>
       <c r="D2"/>
       <c r="E2" s="26"/>
-      <c r="F2" s="98" t="s">
+      <c r="F2" s="96" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="99"/>
+      <c r="G2" s="97"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="26"/>
@@ -6325,10 +6356,10 @@
       <c r="C6" s="28"/>
       <c r="D6"/>
       <c r="E6" s="26"/>
-      <c r="F6" s="100" t="s">
+      <c r="F6" s="98" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="101"/>
+      <c r="G6" s="99"/>
     </row>
     <row r="7" spans="1:7" ht="19.5" customHeight="1" thickBot="1">
       <c r="A7" s="26"/>
@@ -6459,37 +6490,37 @@
       <c r="G15" s="48"/>
     </row>
     <row r="16" spans="1:7" s="49" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A16" s="102" t="s">
+      <c r="A16" s="100" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="102"/>
-      <c r="C16" s="102"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="102"/>
-      <c r="G16" s="102"/>
+      <c r="B16" s="100"/>
+      <c r="C16" s="100"/>
+      <c r="D16" s="100"/>
+      <c r="E16" s="100"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="100"/>
     </row>
     <row r="17" spans="1:7" s="49" customFormat="1" ht="18.75" customHeight="1">
-      <c r="A17" s="103" t="s">
+      <c r="A17" s="101" t="s">
         <v>63</v>
       </c>
-      <c r="B17" s="103"/>
-      <c r="C17" s="103"/>
-      <c r="D17" s="103"/>
-      <c r="E17" s="103"/>
-      <c r="F17" s="103"/>
-      <c r="G17" s="103"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="101"/>
+      <c r="F17" s="101"/>
+      <c r="G17" s="101"/>
     </row>
     <row r="18" spans="1:7" s="49" customFormat="1">
       <c r="A18" s="50" t="s">
         <v>111</v>
       </c>
-      <c r="B18" s="92" t="s">
+      <c r="B18" s="90" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="93"/>
-      <c r="E18" s="94"/>
+      <c r="C18" s="91"/>
+      <c r="D18" s="91"/>
+      <c r="E18" s="92"/>
       <c r="F18" s="51" t="s">
         <v>46</v>
       </c>
@@ -6502,14 +6533,14 @@
       <c r="A19" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="97"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="95"/>
     </row>
     <row r="20" spans="1:7" s="49" customFormat="1">
       <c r="A20" s="54" t="s">
@@ -6574,23 +6605,23 @@
       <c r="A23" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B23" s="89"/>
-      <c r="C23" s="90"/>
-      <c r="D23" s="90"/>
-      <c r="E23" s="90"/>
-      <c r="F23" s="90"/>
-      <c r="G23" s="91"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="88"/>
+      <c r="D23" s="88"/>
+      <c r="E23" s="88"/>
+      <c r="F23" s="88"/>
+      <c r="G23" s="89"/>
     </row>
     <row r="24" spans="1:7" s="49" customFormat="1">
       <c r="A24" s="50" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="92" t="s">
+      <c r="B24" s="90" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="93"/>
-      <c r="D24" s="93"/>
-      <c r="E24" s="94"/>
+      <c r="C24" s="91"/>
+      <c r="D24" s="91"/>
+      <c r="E24" s="92"/>
       <c r="F24" s="51" t="s">
         <v>46</v>
       </c>
@@ -6603,14 +6634,14 @@
       <c r="A25" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B25" s="95" t="s">
+      <c r="B25" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="96"/>
-      <c r="D25" s="96"/>
-      <c r="E25" s="96"/>
-      <c r="F25" s="96"/>
-      <c r="G25" s="97"/>
+      <c r="C25" s="94"/>
+      <c r="D25" s="94"/>
+      <c r="E25" s="94"/>
+      <c r="F25" s="94"/>
+      <c r="G25" s="95"/>
     </row>
     <row r="26" spans="1:7" s="49" customFormat="1">
       <c r="A26" s="54" t="s">
@@ -6690,23 +6721,23 @@
       <c r="A30" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="89"/>
-      <c r="C30" s="90"/>
-      <c r="D30" s="90"/>
-      <c r="E30" s="90"/>
-      <c r="F30" s="90"/>
-      <c r="G30" s="91"/>
+      <c r="B30" s="87"/>
+      <c r="C30" s="88"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="89"/>
     </row>
     <row r="31" spans="1:7" s="49" customFormat="1">
       <c r="A31" s="50" t="s">
         <v>104</v>
       </c>
-      <c r="B31" s="92" t="s">
+      <c r="B31" s="90" t="s">
         <v>72</v>
       </c>
-      <c r="C31" s="93"/>
-      <c r="D31" s="93"/>
-      <c r="E31" s="94"/>
+      <c r="C31" s="91"/>
+      <c r="D31" s="91"/>
+      <c r="E31" s="92"/>
       <c r="F31" s="51" t="s">
         <v>46</v>
       </c>
@@ -6719,14 +6750,14 @@
       <c r="A32" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="95" t="s">
+      <c r="B32" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="96"/>
-      <c r="D32" s="96"/>
-      <c r="E32" s="96"/>
-      <c r="F32" s="96"/>
-      <c r="G32" s="97"/>
+      <c r="C32" s="94"/>
+      <c r="D32" s="94"/>
+      <c r="E32" s="94"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="95"/>
     </row>
     <row r="33" spans="1:7" s="49" customFormat="1">
       <c r="A33" s="54" t="s">
@@ -6823,23 +6854,23 @@
       <c r="A38" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B38" s="89"/>
-      <c r="C38" s="90"/>
-      <c r="D38" s="90"/>
-      <c r="E38" s="90"/>
-      <c r="F38" s="90"/>
-      <c r="G38" s="91"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="88"/>
+      <c r="D38" s="88"/>
+      <c r="E38" s="88"/>
+      <c r="F38" s="88"/>
+      <c r="G38" s="89"/>
     </row>
     <row r="39" spans="1:7" s="49" customFormat="1">
       <c r="A39" s="50" t="s">
         <v>105</v>
       </c>
-      <c r="B39" s="92" t="s">
+      <c r="B39" s="90" t="s">
         <v>71</v>
       </c>
-      <c r="C39" s="93"/>
-      <c r="D39" s="93"/>
-      <c r="E39" s="94"/>
+      <c r="C39" s="91"/>
+      <c r="D39" s="91"/>
+      <c r="E39" s="92"/>
       <c r="F39" s="51" t="s">
         <v>46</v>
       </c>
@@ -6852,14 +6883,14 @@
       <c r="A40" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="95" t="s">
+      <c r="B40" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C40" s="96"/>
-      <c r="D40" s="96"/>
-      <c r="E40" s="96"/>
-      <c r="F40" s="96"/>
-      <c r="G40" s="97"/>
+      <c r="C40" s="94"/>
+      <c r="D40" s="94"/>
+      <c r="E40" s="94"/>
+      <c r="F40" s="94"/>
+      <c r="G40" s="95"/>
     </row>
     <row r="41" spans="1:7" s="49" customFormat="1">
       <c r="A41" s="54" t="s">
@@ -6956,23 +6987,23 @@
       <c r="A46" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B46" s="89"/>
-      <c r="C46" s="90"/>
-      <c r="D46" s="90"/>
-      <c r="E46" s="90"/>
-      <c r="F46" s="90"/>
-      <c r="G46" s="91"/>
+      <c r="B46" s="87"/>
+      <c r="C46" s="88"/>
+      <c r="D46" s="88"/>
+      <c r="E46" s="88"/>
+      <c r="F46" s="88"/>
+      <c r="G46" s="89"/>
     </row>
     <row r="47" spans="1:7" s="49" customFormat="1">
       <c r="A47" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="B47" s="92" t="s">
+      <c r="B47" s="90" t="s">
         <v>68</v>
       </c>
-      <c r="C47" s="93"/>
-      <c r="D47" s="93"/>
-      <c r="E47" s="94"/>
+      <c r="C47" s="91"/>
+      <c r="D47" s="91"/>
+      <c r="E47" s="92"/>
       <c r="F47" s="51" t="s">
         <v>46</v>
       </c>
@@ -6985,14 +7016,14 @@
       <c r="A48" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="95" t="s">
+      <c r="B48" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="96"/>
-      <c r="D48" s="96"/>
-      <c r="E48" s="96"/>
-      <c r="F48" s="96"/>
-      <c r="G48" s="97"/>
+      <c r="C48" s="94"/>
+      <c r="D48" s="94"/>
+      <c r="E48" s="94"/>
+      <c r="F48" s="94"/>
+      <c r="G48" s="95"/>
     </row>
     <row r="49" spans="1:7" s="49" customFormat="1">
       <c r="A49" s="54" t="s">
@@ -7089,23 +7120,23 @@
       <c r="A54" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="89"/>
-      <c r="C54" s="90"/>
-      <c r="D54" s="90"/>
-      <c r="E54" s="90"/>
-      <c r="F54" s="90"/>
-      <c r="G54" s="91"/>
+      <c r="B54" s="87"/>
+      <c r="C54" s="88"/>
+      <c r="D54" s="88"/>
+      <c r="E54" s="88"/>
+      <c r="F54" s="88"/>
+      <c r="G54" s="89"/>
     </row>
     <row r="55" spans="1:7" s="49" customFormat="1">
       <c r="A55" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B55" s="92" t="s">
+      <c r="B55" s="90" t="s">
         <v>69</v>
       </c>
-      <c r="C55" s="93"/>
-      <c r="D55" s="93"/>
-      <c r="E55" s="94"/>
+      <c r="C55" s="91"/>
+      <c r="D55" s="91"/>
+      <c r="E55" s="92"/>
       <c r="F55" s="51" t="s">
         <v>46</v>
       </c>
@@ -7118,14 +7149,14 @@
       <c r="A56" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B56" s="95" t="s">
+      <c r="B56" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C56" s="96"/>
-      <c r="D56" s="96"/>
-      <c r="E56" s="96"/>
-      <c r="F56" s="96"/>
-      <c r="G56" s="97"/>
+      <c r="C56" s="94"/>
+      <c r="D56" s="94"/>
+      <c r="E56" s="94"/>
+      <c r="F56" s="94"/>
+      <c r="G56" s="95"/>
     </row>
     <row r="57" spans="1:7" s="49" customFormat="1">
       <c r="A57" s="54" t="s">
@@ -7222,23 +7253,23 @@
       <c r="A62" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B62" s="89"/>
-      <c r="C62" s="90"/>
-      <c r="D62" s="90"/>
-      <c r="E62" s="90"/>
-      <c r="F62" s="90"/>
-      <c r="G62" s="91"/>
+      <c r="B62" s="87"/>
+      <c r="C62" s="88"/>
+      <c r="D62" s="88"/>
+      <c r="E62" s="88"/>
+      <c r="F62" s="88"/>
+      <c r="G62" s="89"/>
     </row>
     <row r="63" spans="1:7" s="49" customFormat="1">
       <c r="A63" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="B63" s="92" t="s">
+      <c r="B63" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="C63" s="93"/>
-      <c r="D63" s="93"/>
-      <c r="E63" s="94"/>
+      <c r="C63" s="91"/>
+      <c r="D63" s="91"/>
+      <c r="E63" s="92"/>
       <c r="F63" s="51" t="s">
         <v>46</v>
       </c>
@@ -7251,14 +7282,14 @@
       <c r="A64" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B64" s="95" t="s">
+      <c r="B64" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C64" s="96"/>
-      <c r="D64" s="96"/>
-      <c r="E64" s="96"/>
-      <c r="F64" s="96"/>
-      <c r="G64" s="97"/>
+      <c r="C64" s="94"/>
+      <c r="D64" s="94"/>
+      <c r="E64" s="94"/>
+      <c r="F64" s="94"/>
+      <c r="G64" s="95"/>
     </row>
     <row r="65" spans="1:7" s="49" customFormat="1">
       <c r="A65" s="54" t="s">
@@ -7355,23 +7386,23 @@
       <c r="A70" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B70" s="89"/>
-      <c r="C70" s="90"/>
-      <c r="D70" s="90"/>
-      <c r="E70" s="90"/>
-      <c r="F70" s="90"/>
-      <c r="G70" s="91"/>
+      <c r="B70" s="87"/>
+      <c r="C70" s="88"/>
+      <c r="D70" s="88"/>
+      <c r="E70" s="88"/>
+      <c r="F70" s="88"/>
+      <c r="G70" s="89"/>
     </row>
     <row r="71" spans="1:7" s="49" customFormat="1">
       <c r="A71" s="50" t="s">
         <v>132</v>
       </c>
-      <c r="B71" s="92" t="s">
+      <c r="B71" s="90" t="s">
         <v>92</v>
       </c>
-      <c r="C71" s="93"/>
-      <c r="D71" s="93"/>
-      <c r="E71" s="94"/>
+      <c r="C71" s="91"/>
+      <c r="D71" s="91"/>
+      <c r="E71" s="92"/>
       <c r="F71" s="51" t="s">
         <v>46</v>
       </c>
@@ -7384,14 +7415,14 @@
       <c r="A72" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B72" s="95" t="s">
+      <c r="B72" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C72" s="96"/>
-      <c r="D72" s="96"/>
-      <c r="E72" s="96"/>
-      <c r="F72" s="96"/>
-      <c r="G72" s="97"/>
+      <c r="C72" s="94"/>
+      <c r="D72" s="94"/>
+      <c r="E72" s="94"/>
+      <c r="F72" s="94"/>
+      <c r="G72" s="95"/>
     </row>
     <row r="73" spans="1:7" s="49" customFormat="1">
       <c r="A73" s="54" t="s">
@@ -7488,23 +7519,23 @@
       <c r="A78" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B78" s="89"/>
-      <c r="C78" s="90"/>
-      <c r="D78" s="90"/>
-      <c r="E78" s="90"/>
-      <c r="F78" s="90"/>
-      <c r="G78" s="91"/>
+      <c r="B78" s="87"/>
+      <c r="C78" s="88"/>
+      <c r="D78" s="88"/>
+      <c r="E78" s="88"/>
+      <c r="F78" s="88"/>
+      <c r="G78" s="89"/>
     </row>
     <row r="79" spans="1:7" s="49" customFormat="1">
       <c r="A79" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="B79" s="92" t="s">
+      <c r="B79" s="90" t="s">
         <v>80</v>
       </c>
-      <c r="C79" s="93"/>
-      <c r="D79" s="93"/>
-      <c r="E79" s="94"/>
+      <c r="C79" s="91"/>
+      <c r="D79" s="91"/>
+      <c r="E79" s="92"/>
       <c r="F79" s="51" t="s">
         <v>46</v>
       </c>
@@ -7517,14 +7548,14 @@
       <c r="A80" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B80" s="95" t="s">
+      <c r="B80" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C80" s="96"/>
-      <c r="D80" s="96"/>
-      <c r="E80" s="96"/>
-      <c r="F80" s="96"/>
-      <c r="G80" s="97"/>
+      <c r="C80" s="94"/>
+      <c r="D80" s="94"/>
+      <c r="E80" s="94"/>
+      <c r="F80" s="94"/>
+      <c r="G80" s="95"/>
     </row>
     <row r="81" spans="1:7" s="49" customFormat="1">
       <c r="A81" s="54" t="s">
@@ -7706,23 +7737,23 @@
       <c r="A91" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B91" s="89"/>
-      <c r="C91" s="90"/>
-      <c r="D91" s="90"/>
-      <c r="E91" s="90"/>
-      <c r="F91" s="90"/>
-      <c r="G91" s="91"/>
+      <c r="B91" s="87"/>
+      <c r="C91" s="88"/>
+      <c r="D91" s="88"/>
+      <c r="E91" s="88"/>
+      <c r="F91" s="88"/>
+      <c r="G91" s="89"/>
     </row>
     <row r="92" spans="1:7" customFormat="1">
       <c r="A92" s="50" t="s">
         <v>110</v>
       </c>
-      <c r="B92" s="92" t="s">
+      <c r="B92" s="90" t="s">
         <v>90</v>
       </c>
-      <c r="C92" s="93"/>
-      <c r="D92" s="93"/>
-      <c r="E92" s="94"/>
+      <c r="C92" s="91"/>
+      <c r="D92" s="91"/>
+      <c r="E92" s="92"/>
       <c r="F92" s="51" t="s">
         <v>46</v>
       </c>
@@ -7735,14 +7766,14 @@
       <c r="A93" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B93" s="95" t="s">
+      <c r="B93" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C93" s="96"/>
-      <c r="D93" s="96"/>
-      <c r="E93" s="96"/>
-      <c r="F93" s="96"/>
-      <c r="G93" s="97"/>
+      <c r="C93" s="94"/>
+      <c r="D93" s="94"/>
+      <c r="E93" s="94"/>
+      <c r="F93" s="94"/>
+      <c r="G93" s="95"/>
     </row>
     <row r="94" spans="1:7" customFormat="1">
       <c r="A94" s="54" t="s">
@@ -7941,23 +7972,23 @@
       <c r="A105" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B105" s="89"/>
-      <c r="C105" s="90"/>
-      <c r="D105" s="90"/>
-      <c r="E105" s="90"/>
-      <c r="F105" s="90"/>
-      <c r="G105" s="91"/>
+      <c r="B105" s="87"/>
+      <c r="C105" s="88"/>
+      <c r="D105" s="88"/>
+      <c r="E105" s="88"/>
+      <c r="F105" s="88"/>
+      <c r="G105" s="89"/>
     </row>
     <row r="106" spans="1:7" customFormat="1">
       <c r="A106" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="B106" s="92" t="s">
+      <c r="B106" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="C106" s="93"/>
-      <c r="D106" s="93"/>
-      <c r="E106" s="94"/>
+      <c r="C106" s="91"/>
+      <c r="D106" s="91"/>
+      <c r="E106" s="92"/>
       <c r="F106" s="51" t="s">
         <v>46</v>
       </c>
@@ -7970,14 +8001,14 @@
       <c r="A107" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B107" s="95" t="s">
+      <c r="B107" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C107" s="96"/>
-      <c r="D107" s="96"/>
-      <c r="E107" s="96"/>
-      <c r="F107" s="96"/>
-      <c r="G107" s="97"/>
+      <c r="C107" s="94"/>
+      <c r="D107" s="94"/>
+      <c r="E107" s="94"/>
+      <c r="F107" s="94"/>
+      <c r="G107" s="95"/>
     </row>
     <row r="108" spans="1:7">
       <c r="A108" s="54" t="s">
@@ -8159,23 +8190,23 @@
       <c r="A118" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B118" s="89"/>
-      <c r="C118" s="90"/>
-      <c r="D118" s="90"/>
-      <c r="E118" s="90"/>
-      <c r="F118" s="90"/>
-      <c r="G118" s="91"/>
+      <c r="B118" s="87"/>
+      <c r="C118" s="88"/>
+      <c r="D118" s="88"/>
+      <c r="E118" s="88"/>
+      <c r="F118" s="88"/>
+      <c r="G118" s="89"/>
     </row>
     <row r="119" spans="1:8">
       <c r="A119" s="50" t="s">
         <v>168</v>
       </c>
-      <c r="B119" s="92" t="s">
+      <c r="B119" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="C119" s="93"/>
-      <c r="D119" s="93"/>
-      <c r="E119" s="94"/>
+      <c r="C119" s="91"/>
+      <c r="D119" s="91"/>
+      <c r="E119" s="92"/>
       <c r="F119" s="51" t="s">
         <v>46</v>
       </c>
@@ -8188,14 +8219,14 @@
       <c r="A120" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B120" s="95" t="s">
+      <c r="B120" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C120" s="96"/>
-      <c r="D120" s="96"/>
-      <c r="E120" s="96"/>
-      <c r="F120" s="96"/>
-      <c r="G120" s="97"/>
+      <c r="C120" s="94"/>
+      <c r="D120" s="94"/>
+      <c r="E120" s="94"/>
+      <c r="F120" s="94"/>
+      <c r="G120" s="95"/>
       <c r="H120" s="63"/>
     </row>
     <row r="121" spans="1:8">
@@ -8395,23 +8426,23 @@
       <c r="A132" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B132" s="89"/>
-      <c r="C132" s="90"/>
-      <c r="D132" s="90"/>
-      <c r="E132" s="90"/>
-      <c r="F132" s="90"/>
-      <c r="G132" s="91"/>
+      <c r="B132" s="87"/>
+      <c r="C132" s="88"/>
+      <c r="D132" s="88"/>
+      <c r="E132" s="88"/>
+      <c r="F132" s="88"/>
+      <c r="G132" s="89"/>
     </row>
     <row r="133" spans="1:7">
       <c r="A133" s="50" t="s">
         <v>174</v>
       </c>
-      <c r="B133" s="92" t="s">
+      <c r="B133" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="C133" s="93"/>
-      <c r="D133" s="93"/>
-      <c r="E133" s="94"/>
+      <c r="C133" s="91"/>
+      <c r="D133" s="91"/>
+      <c r="E133" s="92"/>
       <c r="F133" s="51" t="s">
         <v>46</v>
       </c>
@@ -8424,14 +8455,14 @@
       <c r="A134" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B134" s="95" t="s">
+      <c r="B134" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C134" s="96"/>
-      <c r="D134" s="96"/>
-      <c r="E134" s="96"/>
-      <c r="F134" s="96"/>
-      <c r="G134" s="97"/>
+      <c r="C134" s="94"/>
+      <c r="D134" s="94"/>
+      <c r="E134" s="94"/>
+      <c r="F134" s="94"/>
+      <c r="G134" s="95"/>
     </row>
     <row r="135" spans="1:7">
       <c r="A135" s="54" t="s">
@@ -8630,23 +8661,23 @@
       <c r="A146" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B146" s="89"/>
-      <c r="C146" s="90"/>
-      <c r="D146" s="90"/>
-      <c r="E146" s="90"/>
-      <c r="F146" s="90"/>
-      <c r="G146" s="91"/>
+      <c r="B146" s="87"/>
+      <c r="C146" s="88"/>
+      <c r="D146" s="88"/>
+      <c r="E146" s="88"/>
+      <c r="F146" s="88"/>
+      <c r="G146" s="89"/>
     </row>
     <row r="147" spans="1:7">
       <c r="A147" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="B147" s="92" t="s">
+      <c r="B147" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="C147" s="93"/>
-      <c r="D147" s="93"/>
-      <c r="E147" s="94"/>
+      <c r="C147" s="91"/>
+      <c r="D147" s="91"/>
+      <c r="E147" s="92"/>
       <c r="F147" s="51" t="s">
         <v>46</v>
       </c>
@@ -8659,14 +8690,14 @@
       <c r="A148" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B148" s="95" t="s">
+      <c r="B148" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C148" s="96"/>
-      <c r="D148" s="96"/>
-      <c r="E148" s="96"/>
-      <c r="F148" s="96"/>
-      <c r="G148" s="97"/>
+      <c r="C148" s="94"/>
+      <c r="D148" s="94"/>
+      <c r="E148" s="94"/>
+      <c r="F148" s="94"/>
+      <c r="G148" s="95"/>
     </row>
     <row r="149" spans="1:7">
       <c r="A149" s="54" t="s">
@@ -8882,23 +8913,23 @@
       <c r="A161" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B161" s="89"/>
-      <c r="C161" s="90"/>
-      <c r="D161" s="90"/>
-      <c r="E161" s="90"/>
-      <c r="F161" s="90"/>
-      <c r="G161" s="91"/>
+      <c r="B161" s="87"/>
+      <c r="C161" s="88"/>
+      <c r="D161" s="88"/>
+      <c r="E161" s="88"/>
+      <c r="F161" s="88"/>
+      <c r="G161" s="89"/>
     </row>
     <row r="162" spans="1:7">
       <c r="A162" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="B162" s="92" t="s">
+      <c r="B162" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="C162" s="93"/>
-      <c r="D162" s="93"/>
-      <c r="E162" s="94"/>
+      <c r="C162" s="91"/>
+      <c r="D162" s="91"/>
+      <c r="E162" s="92"/>
       <c r="F162" s="51" t="s">
         <v>46</v>
       </c>
@@ -8911,14 +8942,14 @@
       <c r="A163" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B163" s="95" t="s">
+      <c r="B163" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C163" s="96"/>
-      <c r="D163" s="96"/>
-      <c r="E163" s="96"/>
-      <c r="F163" s="96"/>
-      <c r="G163" s="97"/>
+      <c r="C163" s="94"/>
+      <c r="D163" s="94"/>
+      <c r="E163" s="94"/>
+      <c r="F163" s="94"/>
+      <c r="G163" s="95"/>
     </row>
     <row r="164" spans="1:7" ht="30.95" customHeight="1">
       <c r="A164" s="54" t="s">
@@ -9117,23 +9148,23 @@
       <c r="A175" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B175" s="89"/>
-      <c r="C175" s="90"/>
-      <c r="D175" s="90"/>
-      <c r="E175" s="90"/>
-      <c r="F175" s="90"/>
-      <c r="G175" s="91"/>
+      <c r="B175" s="87"/>
+      <c r="C175" s="88"/>
+      <c r="D175" s="88"/>
+      <c r="E175" s="88"/>
+      <c r="F175" s="88"/>
+      <c r="G175" s="89"/>
     </row>
     <row r="176" spans="1:7">
       <c r="A176" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="B176" s="92" t="s">
+      <c r="B176" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="C176" s="93"/>
-      <c r="D176" s="93"/>
-      <c r="E176" s="94"/>
+      <c r="C176" s="91"/>
+      <c r="D176" s="91"/>
+      <c r="E176" s="92"/>
       <c r="F176" s="51" t="s">
         <v>46</v>
       </c>
@@ -9146,14 +9177,14 @@
       <c r="A177" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B177" s="95" t="s">
+      <c r="B177" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C177" s="96"/>
-      <c r="D177" s="96"/>
-      <c r="E177" s="96"/>
-      <c r="F177" s="96"/>
-      <c r="G177" s="97"/>
+      <c r="C177" s="94"/>
+      <c r="D177" s="94"/>
+      <c r="E177" s="94"/>
+      <c r="F177" s="94"/>
+      <c r="G177" s="95"/>
     </row>
     <row r="178" spans="1:7">
       <c r="A178" s="54" t="s">
@@ -9369,23 +9400,23 @@
       <c r="A190" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B190" s="89"/>
-      <c r="C190" s="90"/>
-      <c r="D190" s="90"/>
-      <c r="E190" s="90"/>
-      <c r="F190" s="90"/>
-      <c r="G190" s="91"/>
+      <c r="B190" s="87"/>
+      <c r="C190" s="88"/>
+      <c r="D190" s="88"/>
+      <c r="E190" s="88"/>
+      <c r="F190" s="88"/>
+      <c r="G190" s="89"/>
     </row>
     <row r="191" spans="1:7">
       <c r="A191" s="50" t="s">
         <v>202</v>
       </c>
-      <c r="B191" s="92" t="s">
+      <c r="B191" s="90" t="s">
         <v>203</v>
       </c>
-      <c r="C191" s="93"/>
-      <c r="D191" s="93"/>
-      <c r="E191" s="94"/>
+      <c r="C191" s="91"/>
+      <c r="D191" s="91"/>
+      <c r="E191" s="92"/>
       <c r="F191" s="51" t="s">
         <v>46</v>
       </c>
@@ -9398,14 +9429,14 @@
       <c r="A192" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B192" s="95" t="s">
+      <c r="B192" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C192" s="96"/>
-      <c r="D192" s="96"/>
-      <c r="E192" s="96"/>
-      <c r="F192" s="96"/>
-      <c r="G192" s="97"/>
+      <c r="C192" s="94"/>
+      <c r="D192" s="94"/>
+      <c r="E192" s="94"/>
+      <c r="F192" s="94"/>
+      <c r="G192" s="95"/>
     </row>
     <row r="193" spans="1:7">
       <c r="A193" s="54" t="s">
@@ -9689,23 +9720,23 @@
       <c r="A209" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B209" s="89"/>
-      <c r="C209" s="90"/>
-      <c r="D209" s="90"/>
-      <c r="E209" s="90"/>
-      <c r="F209" s="90"/>
-      <c r="G209" s="91"/>
+      <c r="B209" s="87"/>
+      <c r="C209" s="88"/>
+      <c r="D209" s="88"/>
+      <c r="E209" s="88"/>
+      <c r="F209" s="88"/>
+      <c r="G209" s="89"/>
     </row>
     <row r="210" spans="1:7">
       <c r="A210" s="50" t="s">
         <v>213</v>
       </c>
-      <c r="B210" s="92" t="s">
+      <c r="B210" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="C210" s="93"/>
-      <c r="D210" s="93"/>
-      <c r="E210" s="94"/>
+      <c r="C210" s="91"/>
+      <c r="D210" s="91"/>
+      <c r="E210" s="92"/>
       <c r="F210" s="51" t="s">
         <v>46</v>
       </c>
@@ -9718,14 +9749,14 @@
       <c r="A211" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B211" s="95" t="s">
+      <c r="B211" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C211" s="96"/>
-      <c r="D211" s="96"/>
-      <c r="E211" s="96"/>
-      <c r="F211" s="96"/>
-      <c r="G211" s="97"/>
+      <c r="C211" s="94"/>
+      <c r="D211" s="94"/>
+      <c r="E211" s="94"/>
+      <c r="F211" s="94"/>
+      <c r="G211" s="95"/>
     </row>
     <row r="212" spans="1:7">
       <c r="A212" s="54" t="s">
@@ -9856,23 +9887,23 @@
       <c r="A219" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B219" s="89"/>
-      <c r="C219" s="90"/>
-      <c r="D219" s="90"/>
-      <c r="E219" s="90"/>
-      <c r="F219" s="90"/>
-      <c r="G219" s="91"/>
+      <c r="B219" s="87"/>
+      <c r="C219" s="88"/>
+      <c r="D219" s="88"/>
+      <c r="E219" s="88"/>
+      <c r="F219" s="88"/>
+      <c r="G219" s="89"/>
     </row>
     <row r="220" spans="1:7">
       <c r="A220" s="50" t="s">
         <v>219</v>
       </c>
-      <c r="B220" s="92" t="s">
+      <c r="B220" s="90" t="s">
         <v>252</v>
       </c>
-      <c r="C220" s="93"/>
-      <c r="D220" s="93"/>
-      <c r="E220" s="94"/>
+      <c r="C220" s="91"/>
+      <c r="D220" s="91"/>
+      <c r="E220" s="92"/>
       <c r="F220" s="51" t="s">
         <v>46</v>
       </c>
@@ -9885,14 +9916,14 @@
       <c r="A221" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B221" s="95" t="s">
+      <c r="B221" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C221" s="96"/>
-      <c r="D221" s="96"/>
-      <c r="E221" s="96"/>
-      <c r="F221" s="96"/>
-      <c r="G221" s="97"/>
+      <c r="C221" s="94"/>
+      <c r="D221" s="94"/>
+      <c r="E221" s="94"/>
+      <c r="F221" s="94"/>
+      <c r="G221" s="95"/>
     </row>
     <row r="222" spans="1:7">
       <c r="A222" s="54" t="s">
@@ -10080,23 +10111,23 @@
       <c r="A232" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B232" s="89"/>
-      <c r="C232" s="90"/>
-      <c r="D232" s="90"/>
-      <c r="E232" s="90"/>
-      <c r="F232" s="90"/>
-      <c r="G232" s="91"/>
+      <c r="B232" s="87"/>
+      <c r="C232" s="88"/>
+      <c r="D232" s="88"/>
+      <c r="E232" s="88"/>
+      <c r="F232" s="88"/>
+      <c r="G232" s="89"/>
     </row>
     <row r="233" spans="1:7">
       <c r="A233" s="50" t="s">
         <v>221</v>
       </c>
-      <c r="B233" s="92" t="s">
+      <c r="B233" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C233" s="93"/>
-      <c r="D233" s="93"/>
-      <c r="E233" s="94"/>
+      <c r="C233" s="91"/>
+      <c r="D233" s="91"/>
+      <c r="E233" s="92"/>
       <c r="F233" s="51" t="s">
         <v>46</v>
       </c>
@@ -10109,14 +10140,14 @@
       <c r="A234" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B234" s="95" t="s">
+      <c r="B234" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C234" s="96"/>
-      <c r="D234" s="96"/>
-      <c r="E234" s="96"/>
-      <c r="F234" s="96"/>
-      <c r="G234" s="97"/>
+      <c r="C234" s="94"/>
+      <c r="D234" s="94"/>
+      <c r="E234" s="94"/>
+      <c r="F234" s="94"/>
+      <c r="G234" s="95"/>
     </row>
     <row r="235" spans="1:7">
       <c r="A235" s="54" t="s">
@@ -10247,23 +10278,23 @@
       <c r="A242" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B242" s="89"/>
-      <c r="C242" s="90"/>
-      <c r="D242" s="90"/>
-      <c r="E242" s="90"/>
-      <c r="F242" s="90"/>
-      <c r="G242" s="91"/>
+      <c r="B242" s="87"/>
+      <c r="C242" s="88"/>
+      <c r="D242" s="88"/>
+      <c r="E242" s="88"/>
+      <c r="F242" s="88"/>
+      <c r="G242" s="89"/>
     </row>
     <row r="243" spans="1:7">
       <c r="A243" s="50" t="s">
         <v>228</v>
       </c>
-      <c r="B243" s="92" t="s">
+      <c r="B243" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="C243" s="93"/>
-      <c r="D243" s="93"/>
-      <c r="E243" s="94"/>
+      <c r="C243" s="91"/>
+      <c r="D243" s="91"/>
+      <c r="E243" s="92"/>
       <c r="F243" s="51" t="s">
         <v>46</v>
       </c>
@@ -10276,14 +10307,14 @@
       <c r="A244" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B244" s="95" t="s">
+      <c r="B244" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C244" s="96"/>
-      <c r="D244" s="96"/>
-      <c r="E244" s="96"/>
-      <c r="F244" s="96"/>
-      <c r="G244" s="97"/>
+      <c r="C244" s="94"/>
+      <c r="D244" s="94"/>
+      <c r="E244" s="94"/>
+      <c r="F244" s="94"/>
+      <c r="G244" s="95"/>
     </row>
     <row r="245" spans="1:7">
       <c r="A245" s="54" t="s">
@@ -10397,23 +10428,23 @@
       <c r="A251" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B251" s="89"/>
-      <c r="C251" s="90"/>
-      <c r="D251" s="90"/>
-      <c r="E251" s="90"/>
-      <c r="F251" s="90"/>
-      <c r="G251" s="91"/>
+      <c r="B251" s="87"/>
+      <c r="C251" s="88"/>
+      <c r="D251" s="88"/>
+      <c r="E251" s="88"/>
+      <c r="F251" s="88"/>
+      <c r="G251" s="89"/>
     </row>
     <row r="252" spans="1:7">
       <c r="A252" s="50" t="s">
         <v>240</v>
       </c>
-      <c r="B252" s="92" t="s">
+      <c r="B252" s="90" t="s">
         <v>241</v>
       </c>
-      <c r="C252" s="93"/>
-      <c r="D252" s="93"/>
-      <c r="E252" s="94"/>
+      <c r="C252" s="91"/>
+      <c r="D252" s="91"/>
+      <c r="E252" s="92"/>
       <c r="F252" s="51" t="s">
         <v>46</v>
       </c>
@@ -10426,14 +10457,14 @@
       <c r="A253" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B253" s="95" t="s">
+      <c r="B253" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C253" s="96"/>
-      <c r="D253" s="96"/>
-      <c r="E253" s="96"/>
-      <c r="F253" s="96"/>
-      <c r="G253" s="97"/>
+      <c r="C253" s="94"/>
+      <c r="D253" s="94"/>
+      <c r="E253" s="94"/>
+      <c r="F253" s="94"/>
+      <c r="G253" s="95"/>
     </row>
     <row r="254" spans="1:7">
       <c r="A254" s="54" t="s">
@@ -10530,23 +10561,23 @@
       <c r="A259" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B259" s="89"/>
-      <c r="C259" s="90"/>
-      <c r="D259" s="90"/>
-      <c r="E259" s="90"/>
-      <c r="F259" s="90"/>
-      <c r="G259" s="91"/>
+      <c r="B259" s="87"/>
+      <c r="C259" s="88"/>
+      <c r="D259" s="88"/>
+      <c r="E259" s="88"/>
+      <c r="F259" s="88"/>
+      <c r="G259" s="89"/>
     </row>
     <row r="260" spans="1:7">
       <c r="A260" s="50" t="s">
         <v>260</v>
       </c>
-      <c r="B260" s="92" t="s">
+      <c r="B260" s="90" t="s">
         <v>258</v>
       </c>
-      <c r="C260" s="93"/>
-      <c r="D260" s="93"/>
-      <c r="E260" s="94"/>
+      <c r="C260" s="91"/>
+      <c r="D260" s="91"/>
+      <c r="E260" s="92"/>
       <c r="F260" s="51" t="s">
         <v>46</v>
       </c>
@@ -10559,14 +10590,14 @@
       <c r="A261" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B261" s="95" t="s">
+      <c r="B261" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C261" s="96"/>
-      <c r="D261" s="96"/>
-      <c r="E261" s="96"/>
-      <c r="F261" s="96"/>
-      <c r="G261" s="97"/>
+      <c r="C261" s="94"/>
+      <c r="D261" s="94"/>
+      <c r="E261" s="94"/>
+      <c r="F261" s="94"/>
+      <c r="G261" s="95"/>
     </row>
     <row r="262" spans="1:7">
       <c r="A262" s="54" t="s">
@@ -10678,29 +10709,29 @@
       <c r="F267" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="G267" s="79"/>
+      <c r="G267" s="76"/>
     </row>
     <row r="268" spans="1:7">
       <c r="A268" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B268" s="89"/>
-      <c r="C268" s="90"/>
-      <c r="D268" s="90"/>
-      <c r="E268" s="90"/>
-      <c r="F268" s="90"/>
-      <c r="G268" s="91"/>
+      <c r="B268" s="87"/>
+      <c r="C268" s="88"/>
+      <c r="D268" s="88"/>
+      <c r="E268" s="88"/>
+      <c r="F268" s="88"/>
+      <c r="G268" s="89"/>
     </row>
     <row r="269" spans="1:7" customFormat="1">
       <c r="A269" s="50" t="s">
+        <v>292</v>
+      </c>
+      <c r="B269" s="90" t="s">
         <v>268</v>
       </c>
-      <c r="B269" s="92" t="s">
-        <v>269</v>
-      </c>
-      <c r="C269" s="93"/>
-      <c r="D269" s="93"/>
-      <c r="E269" s="94"/>
+      <c r="C269" s="91"/>
+      <c r="D269" s="91"/>
+      <c r="E269" s="92"/>
       <c r="F269" s="51" t="s">
         <v>46</v>
       </c>
@@ -10713,14 +10744,14 @@
       <c r="A270" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B270" s="95" t="s">
+      <c r="B270" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C270" s="96"/>
-      <c r="D270" s="96"/>
-      <c r="E270" s="96"/>
-      <c r="F270" s="96"/>
-      <c r="G270" s="97"/>
+      <c r="C270" s="94"/>
+      <c r="D270" s="94"/>
+      <c r="E270" s="94"/>
+      <c r="F270" s="94"/>
+      <c r="G270" s="95"/>
     </row>
     <row r="271" spans="1:7" customFormat="1">
       <c r="A271" s="54" t="s">
@@ -10753,10 +10784,10 @@
         <v>56</v>
       </c>
       <c r="C272" s="57" t="s">
+        <v>269</v>
+      </c>
+      <c r="D272" s="57" t="s">
         <v>270</v>
-      </c>
-      <c r="D272" s="57" t="s">
-        <v>271</v>
       </c>
       <c r="E272" s="57"/>
       <c r="F272" s="58" t="s">
@@ -10769,10 +10800,10 @@
         <v>2</v>
       </c>
       <c r="B273" s="56" t="s">
+        <v>271</v>
+      </c>
+      <c r="C273" s="57" t="s">
         <v>272</v>
-      </c>
-      <c r="C273" s="57" t="s">
-        <v>273</v>
       </c>
       <c r="D273" s="57"/>
       <c r="E273" s="57"/>
@@ -10786,10 +10817,10 @@
         <v>3</v>
       </c>
       <c r="B274" s="56" t="s">
+        <v>273</v>
+      </c>
+      <c r="C274" s="57" t="s">
         <v>274</v>
-      </c>
-      <c r="C274" s="57" t="s">
-        <v>275</v>
       </c>
       <c r="D274" s="57"/>
       <c r="E274" s="57"/>
@@ -10803,10 +10834,10 @@
         <v>4</v>
       </c>
       <c r="B275" s="56" t="s">
+        <v>275</v>
+      </c>
+      <c r="C275" s="57" t="s">
         <v>276</v>
-      </c>
-      <c r="C275" s="57" t="s">
-        <v>277</v>
       </c>
       <c r="D275" s="57"/>
       <c r="E275" s="57"/>
@@ -10819,23 +10850,23 @@
       <c r="A276" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B276" s="89"/>
-      <c r="C276" s="90"/>
-      <c r="D276" s="90"/>
-      <c r="E276" s="90"/>
-      <c r="F276" s="90"/>
-      <c r="G276" s="91"/>
+      <c r="B276" s="87"/>
+      <c r="C276" s="88"/>
+      <c r="D276" s="88"/>
+      <c r="E276" s="88"/>
+      <c r="F276" s="88"/>
+      <c r="G276" s="89"/>
     </row>
     <row r="277" spans="1:7" customFormat="1">
       <c r="A277" s="50" t="s">
-        <v>278</v>
-      </c>
-      <c r="B277" s="92" t="s">
-        <v>279</v>
-      </c>
-      <c r="C277" s="93"/>
-      <c r="D277" s="93"/>
-      <c r="E277" s="94"/>
+        <v>293</v>
+      </c>
+      <c r="B277" s="90" t="s">
+        <v>277</v>
+      </c>
+      <c r="C277" s="91"/>
+      <c r="D277" s="91"/>
+      <c r="E277" s="92"/>
       <c r="F277" s="51" t="s">
         <v>46</v>
       </c>
@@ -10848,14 +10879,14 @@
       <c r="A278" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B278" s="95" t="s">
+      <c r="B278" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C278" s="96"/>
-      <c r="D278" s="96"/>
-      <c r="E278" s="96"/>
-      <c r="F278" s="96"/>
-      <c r="G278" s="97"/>
+      <c r="C278" s="94"/>
+      <c r="D278" s="94"/>
+      <c r="E278" s="94"/>
+      <c r="F278" s="94"/>
+      <c r="G278" s="95"/>
     </row>
     <row r="279" spans="1:7" customFormat="1" ht="45.75" customHeight="1">
       <c r="A279" s="54" t="s">
@@ -10888,10 +10919,10 @@
         <v>56</v>
       </c>
       <c r="C280" s="57" t="s">
+        <v>269</v>
+      </c>
+      <c r="D280" s="57" t="s">
         <v>270</v>
-      </c>
-      <c r="D280" s="57" t="s">
-        <v>271</v>
       </c>
       <c r="E280" s="57"/>
       <c r="F280" s="58" t="s">
@@ -10904,10 +10935,10 @@
         <v>2</v>
       </c>
       <c r="B281" s="56" t="s">
+        <v>271</v>
+      </c>
+      <c r="C281" s="57" t="s">
         <v>272</v>
-      </c>
-      <c r="C281" s="57" t="s">
-        <v>273</v>
       </c>
       <c r="D281" s="57"/>
       <c r="E281" s="57"/>
@@ -10921,10 +10952,10 @@
         <v>3</v>
       </c>
       <c r="B282" s="56" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C282" s="57" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D282" s="57"/>
       <c r="E282" s="57"/>
@@ -10938,10 +10969,10 @@
         <v>4</v>
       </c>
       <c r="B283" s="56" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C283" s="57" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D283" s="57"/>
       <c r="E283" s="57"/>
@@ -10955,10 +10986,10 @@
         <v>5</v>
       </c>
       <c r="B284" s="56" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="C284" s="57" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D284" s="57"/>
       <c r="E284" s="57"/>
@@ -10971,23 +11002,23 @@
       <c r="A285" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B285" s="89"/>
-      <c r="C285" s="90"/>
-      <c r="D285" s="90"/>
-      <c r="E285" s="90"/>
-      <c r="F285" s="90"/>
-      <c r="G285" s="91"/>
+      <c r="B285" s="87"/>
+      <c r="C285" s="88"/>
+      <c r="D285" s="88"/>
+      <c r="E285" s="88"/>
+      <c r="F285" s="88"/>
+      <c r="G285" s="89"/>
     </row>
     <row r="286" spans="1:7" customFormat="1">
       <c r="A286" s="50" t="s">
-        <v>285</v>
-      </c>
-      <c r="B286" s="92" t="s">
-        <v>286</v>
-      </c>
-      <c r="C286" s="93"/>
-      <c r="D286" s="93"/>
-      <c r="E286" s="94"/>
+        <v>294</v>
+      </c>
+      <c r="B286" s="90" t="s">
+        <v>283</v>
+      </c>
+      <c r="C286" s="91"/>
+      <c r="D286" s="91"/>
+      <c r="E286" s="92"/>
       <c r="F286" s="51" t="s">
         <v>46</v>
       </c>
@@ -11000,14 +11031,14 @@
       <c r="A287" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="B287" s="95" t="s">
+      <c r="B287" s="93" t="s">
         <v>48</v>
       </c>
-      <c r="C287" s="96"/>
-      <c r="D287" s="96"/>
-      <c r="E287" s="96"/>
-      <c r="F287" s="96"/>
-      <c r="G287" s="97"/>
+      <c r="C287" s="94"/>
+      <c r="D287" s="94"/>
+      <c r="E287" s="94"/>
+      <c r="F287" s="94"/>
+      <c r="G287" s="95"/>
     </row>
     <row r="288" spans="1:7" customFormat="1">
       <c r="A288" s="54" t="s">
@@ -11040,10 +11071,10 @@
         <v>56</v>
       </c>
       <c r="C289" s="57" t="s">
+        <v>269</v>
+      </c>
+      <c r="D289" s="57" t="s">
         <v>270</v>
-      </c>
-      <c r="D289" s="57" t="s">
-        <v>271</v>
       </c>
       <c r="E289" s="57"/>
       <c r="F289" s="58" t="s">
@@ -11056,10 +11087,10 @@
         <v>2</v>
       </c>
       <c r="B290" s="56" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C290" s="57" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="D290" s="57"/>
       <c r="E290" s="57"/>
@@ -11073,10 +11104,10 @@
         <v>3</v>
       </c>
       <c r="B291" s="56" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C291" s="57" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D291" s="57"/>
       <c r="E291" s="57"/>
@@ -11085,15 +11116,15 @@
       </c>
       <c r="G291" s="59"/>
     </row>
-    <row r="292" spans="1:7" s="104" customFormat="1" ht="91.5" customHeight="1">
+    <row r="292" spans="1:7" s="77" customFormat="1" ht="91.5" customHeight="1">
       <c r="A292" s="55">
         <v>4</v>
       </c>
       <c r="B292" s="56" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C292" s="57" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D292" s="57"/>
       <c r="E292" s="57"/>
@@ -11106,12 +11137,12 @@
       <c r="A293" s="60" t="s">
         <v>57</v>
       </c>
-      <c r="B293" s="89"/>
-      <c r="C293" s="90"/>
-      <c r="D293" s="90"/>
-      <c r="E293" s="90"/>
-      <c r="F293" s="90"/>
-      <c r="G293" s="91"/>
+      <c r="B293" s="87"/>
+      <c r="C293" s="88"/>
+      <c r="D293" s="88"/>
+      <c r="E293" s="88"/>
+      <c r="F293" s="88"/>
+      <c r="G293" s="89"/>
     </row>
     <row r="294" spans="1:7">
       <c r="A294"/>
@@ -17115,15 +17146,63 @@
     </row>
   </sheetData>
   <mergeCells count="82">
-    <mergeCell ref="B285:G285"/>
-    <mergeCell ref="B286:E286"/>
-    <mergeCell ref="B287:G287"/>
-    <mergeCell ref="B293:G293"/>
-    <mergeCell ref="B269:E269"/>
-    <mergeCell ref="B270:G270"/>
-    <mergeCell ref="B276:G276"/>
-    <mergeCell ref="B277:E277"/>
-    <mergeCell ref="B278:G278"/>
+    <mergeCell ref="B259:G259"/>
+    <mergeCell ref="B243:E243"/>
+    <mergeCell ref="B244:G244"/>
+    <mergeCell ref="B251:G251"/>
+    <mergeCell ref="B252:E252"/>
+    <mergeCell ref="B253:G253"/>
+    <mergeCell ref="B221:G221"/>
+    <mergeCell ref="B232:G232"/>
+    <mergeCell ref="B233:E233"/>
+    <mergeCell ref="B234:G234"/>
+    <mergeCell ref="B242:G242"/>
+    <mergeCell ref="B209:G209"/>
+    <mergeCell ref="B210:E210"/>
+    <mergeCell ref="B211:G211"/>
+    <mergeCell ref="B219:G219"/>
+    <mergeCell ref="B220:E220"/>
+    <mergeCell ref="B176:E176"/>
+    <mergeCell ref="B177:G177"/>
+    <mergeCell ref="B190:G190"/>
+    <mergeCell ref="B191:E191"/>
+    <mergeCell ref="B192:G192"/>
+    <mergeCell ref="B148:G148"/>
+    <mergeCell ref="B161:G161"/>
+    <mergeCell ref="B162:E162"/>
+    <mergeCell ref="B163:G163"/>
+    <mergeCell ref="B175:G175"/>
+    <mergeCell ref="B132:G132"/>
+    <mergeCell ref="B133:E133"/>
+    <mergeCell ref="B134:G134"/>
+    <mergeCell ref="B146:G146"/>
+    <mergeCell ref="B147:E147"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="A16:G16"/>
+    <mergeCell ref="A17:G17"/>
+    <mergeCell ref="B18:E18"/>
+    <mergeCell ref="B19:G19"/>
+    <mergeCell ref="B23:G23"/>
+    <mergeCell ref="B24:E24"/>
+    <mergeCell ref="B56:G56"/>
+    <mergeCell ref="B30:G30"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B32:G32"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="B40:G40"/>
+    <mergeCell ref="B46:G46"/>
+    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B48:G48"/>
+    <mergeCell ref="B54:G54"/>
+    <mergeCell ref="B55:E55"/>
+    <mergeCell ref="B62:G62"/>
+    <mergeCell ref="B63:E63"/>
+    <mergeCell ref="B64:G64"/>
+    <mergeCell ref="B71:E71"/>
+    <mergeCell ref="B72:G72"/>
     <mergeCell ref="B260:E260"/>
     <mergeCell ref="B261:G261"/>
     <mergeCell ref="B268:G268"/>
@@ -17140,63 +17219,15 @@
     <mergeCell ref="B118:G118"/>
     <mergeCell ref="B119:E119"/>
     <mergeCell ref="B120:G120"/>
-    <mergeCell ref="B62:G62"/>
-    <mergeCell ref="B63:E63"/>
-    <mergeCell ref="B64:G64"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="B72:G72"/>
-    <mergeCell ref="B56:G56"/>
-    <mergeCell ref="B30:G30"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B32:G32"/>
-    <mergeCell ref="B38:G38"/>
-    <mergeCell ref="B39:E39"/>
-    <mergeCell ref="B40:G40"/>
-    <mergeCell ref="B46:G46"/>
-    <mergeCell ref="B47:E47"/>
-    <mergeCell ref="B48:G48"/>
-    <mergeCell ref="B54:G54"/>
-    <mergeCell ref="B55:E55"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="A16:G16"/>
-    <mergeCell ref="A17:G17"/>
-    <mergeCell ref="B18:E18"/>
-    <mergeCell ref="B19:G19"/>
-    <mergeCell ref="B23:G23"/>
-    <mergeCell ref="B24:E24"/>
-    <mergeCell ref="B132:G132"/>
-    <mergeCell ref="B133:E133"/>
-    <mergeCell ref="B134:G134"/>
-    <mergeCell ref="B146:G146"/>
-    <mergeCell ref="B147:E147"/>
-    <mergeCell ref="B148:G148"/>
-    <mergeCell ref="B161:G161"/>
-    <mergeCell ref="B162:E162"/>
-    <mergeCell ref="B163:G163"/>
-    <mergeCell ref="B175:G175"/>
-    <mergeCell ref="B176:E176"/>
-    <mergeCell ref="B177:G177"/>
-    <mergeCell ref="B190:G190"/>
-    <mergeCell ref="B191:E191"/>
-    <mergeCell ref="B192:G192"/>
-    <mergeCell ref="B209:G209"/>
-    <mergeCell ref="B210:E210"/>
-    <mergeCell ref="B211:G211"/>
-    <mergeCell ref="B219:G219"/>
-    <mergeCell ref="B220:E220"/>
-    <mergeCell ref="B221:G221"/>
-    <mergeCell ref="B232:G232"/>
-    <mergeCell ref="B233:E233"/>
-    <mergeCell ref="B234:G234"/>
-    <mergeCell ref="B242:G242"/>
-    <mergeCell ref="B259:G259"/>
-    <mergeCell ref="B243:E243"/>
-    <mergeCell ref="B244:G244"/>
-    <mergeCell ref="B251:G251"/>
-    <mergeCell ref="B252:E252"/>
-    <mergeCell ref="B253:G253"/>
+    <mergeCell ref="B285:G285"/>
+    <mergeCell ref="B286:E286"/>
+    <mergeCell ref="B287:G287"/>
+    <mergeCell ref="B293:G293"/>
+    <mergeCell ref="B269:E269"/>
+    <mergeCell ref="B270:G270"/>
+    <mergeCell ref="B276:G276"/>
+    <mergeCell ref="B277:E277"/>
+    <mergeCell ref="B278:G278"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" showErrorMessage="1" promptTitle="Valid values include:" prompt="_x000a_" sqref="F443:F445 F450:F456 F669:F671 F659:F664 F461:F470 F475:F478 F483:F488 F493:F501 F506:F515 F520:F530 F535:F545 F561:F567 F589:F591 F550:F556 F572:F578 F583:F584 F596:F602 F607:F613 F629:F631 F618:F624 F636:F639 F644:F646 F651:F654 F21:F22 F50:F53 F34:F37 F27:F29 F82:F90 F42:F45 F66:F69 F74:F77 F58:F61 F95:F104 F109:F117 F122:F131 F136:F145 F150:F160 F165:F174 F179:F189 F194:F208 F213:F218 F223:F231 F236:F241 F246:F250 F255:F258 F263:F267 F272:F275 F280:F284 F289:F292">

</xml_diff>